<commit_message>
ALMOST finished with lambda for continuous traits <3
</commit_message>
<xml_diff>
--- a/Results/Update Coastal_RESULTS.xlsx
+++ b/Results/Update Coastal_RESULTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/emgarris_calpoly_edu/Documents/R_Projects/CoastalBirdsUPDATE/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="257" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81AB1744-ADE2-43B1-BAB3-39C5206582FE}"/>
+  <xr:revisionPtr revIDLastSave="276" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6C1714C-1228-49C3-8AED-28882C8BD6A0}"/>
   <bookViews>
     <workbookView xWindow="7870" yWindow="290" windowWidth="11320" windowHeight="9260" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="62">
   <si>
     <t>Index used</t>
   </si>
@@ -209,6 +209,12 @@
   <si>
     <t xml:space="preserve">ordinal?????? Try </t>
   </si>
+  <si>
+    <t>~0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">????? Revisit </t>
+  </si>
 </sst>
 </file>
 
@@ -271,7 +277,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -335,12 +341,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -510,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -636,12 +636,6 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -651,35 +645,34 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1042,20 +1035,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65DA1016-BA3D-4155-BE4B-26BD850BD445}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.36328125" customWidth="1"/>
     <col min="3" max="3" width="13.81640625" customWidth="1"/>
-    <col min="4" max="4" width="32" style="47" customWidth="1"/>
+    <col min="4" max="4" width="32" style="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
@@ -1069,15 +1062,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="49"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="47"/>
       <c r="D2" s="16"/>
     </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="19" t="s">
         <v>30</v>
       </c>
@@ -1089,7 +1082,7 @@
       </c>
       <c r="D3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="20" t="s">
         <v>31</v>
       </c>
@@ -1101,90 +1094,99 @@
       </c>
       <c r="D4" s="16"/>
     </row>
-    <row r="5" spans="1:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="50">
+      <c r="B5" s="12">
         <v>0.84499999999999997</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="11" t="s">
         <v>29</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="50">
+      <c r="B6" s="12">
         <v>0.86</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="11" t="s">
         <v>29</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="44.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" ht="44.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="50">
+      <c r="B7" s="12">
         <v>0.82799999999999996</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="11" t="s">
         <v>29</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="59">
+      <c r="B8" s="52">
         <v>0.91200000000000003</v>
       </c>
-      <c r="C8" s="60" t="s">
+      <c r="C8" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="58" t="s">
+      <c r="D8" s="51" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="52"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="56"/>
-    </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="53">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="C9" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="50"/>
+    </row>
+    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="56"/>
-    </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="55">
+        <v>0.876</v>
+      </c>
+      <c r="C10" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="48"/>
+    </row>
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="56"/>
-    </row>
-    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="55">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="C11" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="48"/>
+    </row>
+    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="25" t="s">
         <v>42</v>
       </c>
@@ -1194,12 +1196,11 @@
       <c r="C12" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="56"/>
-    </row>
-    <row r="13" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="13" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="26" t="s">
         <v>45</v>
       </c>
@@ -1209,12 +1210,11 @@
       <c r="C13" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="54" t="s">
+      <c r="D13" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="56"/>
-    </row>
-    <row r="14" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="14" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="26" t="s">
         <v>46</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="26" t="s">
         <v>47</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="26" t="s">
         <v>48</v>
       </c>
@@ -1260,11 +1260,11 @@
       <c r="A17" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>43</v>
+      <c r="B17" s="11">
+        <v>0.876</v>
+      </c>
+      <c r="C17" s="51" t="s">
+        <v>29</v>
       </c>
       <c r="D17" s="16" t="s">
         <v>59</v>
@@ -1274,24 +1274,30 @@
       <c r="A18" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="30"/>
+      <c r="B18" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="43">
+        <v>1</v>
+      </c>
+      <c r="D18" s="57" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="19" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
       <c r="D19" s="30"/>
     </row>
     <row r="20" spans="1:4" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="46"/>
-      <c r="C20" s="46"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
       <c r="D20" s="11" t="s">
         <v>58</v>
       </c>
@@ -1300,8 +1306,8 @@
       <c r="A21" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="46"/>
-      <c r="C21" s="46"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
       <c r="D21" s="11" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
halfway through diet - committ before dinner break!
</commit_message>
<xml_diff>
--- a/Results/Update Coastal_RESULTS.xlsx
+++ b/Results/Update Coastal_RESULTS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/emgarris_calpoly_edu/Documents/R_Projects/CoastalBirdsUPDATE/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="540" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64243A7A-9FE2-4607-BC16-8D0B7AF6AE26}"/>
+  <xr:revisionPtr revIDLastSave="621" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D72D7546-D26E-4E7E-857A-7D7696B0FE0B}"/>
   <bookViews>
-    <workbookView xWindow="7890" yWindow="950" windowWidth="11320" windowHeight="9260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sensory" sheetId="4" r:id="rId1"/>
@@ -21,17 +21,28 @@
     <sheet name="Social" sheetId="13" r:id="rId6"/>
     <sheet name="Body Mass" sheetId="14" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="42">
   <si>
     <t>Index used</t>
   </si>
@@ -136,6 +147,27 @@
   </si>
   <si>
     <t>low collinearity, normal q-q looks good but trails off a bit at ends, good normality of residuals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">normal q-q looks ok, trails off at end, low collinearity </t>
+  </si>
+  <si>
+    <t>histograms of binomial distributions and q-q-q look fine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001707	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">low collinearity, normal q-q plot trails off on ends, histogram of residuals slightly skewed right (not concerning though) </t>
+  </si>
+  <si>
+    <t>low collinearity, normality of residuals (q-q) trails off at ends</t>
+  </si>
+  <si>
+    <t xml:space="preserve">each binomial distribution looks very different - much more 0 = UN species </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.01373	</t>
   </si>
 </sst>
 </file>
@@ -144,7 +176,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="0.000E+00"/>
+    <numFmt numFmtId="165" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -290,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -309,11 +341,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -329,27 +359,24 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -360,7 +387,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,7 +680,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="13.54296875" style="38" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" style="33" customWidth="1"/>
     <col min="6" max="6" width="11.7265625" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.7265625" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
@@ -674,37 +701,37 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="14" t="s">
         <v>11</v>
       </c>
       <c r="O1" s="3" t="s">
@@ -712,7 +739,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -721,37 +748,37 @@
       <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="30" t="s">
         <v>15</v>
       </c>
       <c r="E2" s="5">
         <v>237</v>
       </c>
-      <c r="F2" s="18">
+      <c r="F2" s="16">
         <v>0.26300000000000001</v>
       </c>
-      <c r="G2" s="18">
+      <c r="G2" s="16">
         <v>0.61</v>
       </c>
-      <c r="H2" s="18">
+      <c r="H2" s="16">
         <v>0.432</v>
       </c>
-      <c r="I2" s="18">
+      <c r="I2" s="16">
         <v>0.66600000000000004</v>
       </c>
-      <c r="J2" s="18">
+      <c r="J2" s="16">
         <v>-0.93200000000000005</v>
       </c>
-      <c r="K2" s="18">
+      <c r="K2" s="16">
         <v>1.458</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="L2" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="18" t="s">
+      <c r="M2" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="19">
+      <c r="N2" s="17">
         <v>0</v>
       </c>
       <c r="O2" s="5" t="s">
@@ -759,7 +786,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -768,7 +795,7 @@
       <c r="C3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="31" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="6">
@@ -806,7 +833,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -815,58 +842,49 @@
       <c r="C4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="32" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="9">
         <v>38</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="18">
         <v>-1.381418</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="19">
         <v>1.3702799999999999</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="19">
         <v>1.0081</v>
       </c>
-      <c r="I4" s="21">
+      <c r="I4" s="19">
         <v>0.32029999999999997</v>
       </c>
-      <c r="J4" s="21">
+      <c r="J4" s="19">
         <v>-4.0671163000000004</v>
       </c>
-      <c r="K4" s="21">
+      <c r="K4" s="19">
         <v>1.3042807000000001</v>
       </c>
-      <c r="L4" s="21">
+      <c r="L4" s="19">
         <v>3.6850000000000001E-2</v>
       </c>
-      <c r="M4" s="21">
+      <c r="M4" s="19">
         <v>-1.8190000000000001E-2</v>
       </c>
-      <c r="N4" s="21">
+      <c r="N4" s="19">
         <v>0</v>
       </c>
       <c r="O4" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="14"/>
-      <c r="D5" s="39"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" s="13"/>
+      <c r="F5" s="20"/>
     </row>
     <row r="6" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -875,37 +893,37 @@
       <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="26">
         <v>202</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="22">
         <v>-4.2299999999999998E-5</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="22">
         <v>4.07E-5</v>
       </c>
-      <c r="H6" s="24">
+      <c r="H6" s="21">
         <v>-1.0410079999999999</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="16">
         <v>0.29909999999999998</v>
       </c>
-      <c r="J6" s="26">
+      <c r="J6" s="23">
         <v>1.220738E-4</v>
       </c>
-      <c r="K6" s="26">
+      <c r="K6" s="23">
         <v>3.7381359999999998E-5</v>
       </c>
-      <c r="L6" s="18" t="s">
+      <c r="L6" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="M6" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="N6" s="19">
+      <c r="N6" s="17">
         <v>0.72</v>
       </c>
       <c r="O6" s="5" t="s">
@@ -913,7 +931,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -922,16 +940,16 @@
       <c r="C7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="6">
         <v>68</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="24">
         <v>-2.9899999999999998E-5</v>
       </c>
-      <c r="G7" s="27">
+      <c r="G7" s="24">
         <v>1.5410000000000001E-4</v>
       </c>
       <c r="H7" s="7">
@@ -940,10 +958,10 @@
       <c r="I7" s="7">
         <v>0.84689999999999999</v>
       </c>
-      <c r="J7" s="28">
+      <c r="J7" s="25">
         <v>-3.3183289999999999E-4</v>
       </c>
-      <c r="K7" s="28">
+      <c r="K7" s="25">
         <v>2.7208810000000001E-4</v>
       </c>
       <c r="L7" s="8" t="s">
@@ -960,7 +978,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -969,37 +987,37 @@
       <c r="C8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="9">
         <v>129</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="19">
         <v>4.5936999999999997E-5</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="27">
         <v>4.1950999999999999E-5</v>
       </c>
-      <c r="H8" s="32">
+      <c r="H8" s="27">
         <v>1.095</v>
       </c>
-      <c r="I8" s="21">
+      <c r="I8" s="19">
         <v>0.27560000000000001</v>
       </c>
-      <c r="J8" s="32">
+      <c r="J8" s="27">
         <v>-3.6284820000000003E-5</v>
       </c>
-      <c r="K8" s="32">
+      <c r="K8" s="27">
         <v>1.2815870000000001E-4</v>
       </c>
-      <c r="L8" s="21">
+      <c r="L8" s="19">
         <v>1.111E-2</v>
       </c>
-      <c r="M8" s="21">
+      <c r="M8" s="19">
         <v>-4.5820000000000001E-3</v>
       </c>
-      <c r="N8" s="32">
+      <c r="N8" s="27">
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="O8" s="9" t="s">
@@ -1007,10 +1025,10 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A9" s="15"/>
+      <c r="A9" s="13"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" s="15"/>
+      <c r="A10" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1022,15 +1040,23 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="18.26953125" style="38" customWidth="1"/>
+    <col min="4" max="4" width="18.26953125" style="33" customWidth="1"/>
+    <col min="6" max="6" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.7265625" style="4"/>
+    <col min="10" max="10" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7265625" style="4"/>
+    <col min="13" max="13" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.08984375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1040,37 +1066,37 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="14" t="s">
         <v>11</v>
       </c>
       <c r="O1" s="3" t="s">
@@ -1078,7 +1104,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1087,37 +1113,37 @@
       <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="30" t="s">
         <v>31</v>
       </c>
       <c r="E2" s="5">
         <v>798</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="23">
         <v>-4.0269999999999998E-4</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="23">
         <v>8.9329999999999998E-4</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="17">
         <v>-0.45077200000000001</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="17">
         <v>0.65229999999999999</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="23">
         <v>-2.15351E-3</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="23">
         <v>1.3481610000000001E-3</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="5">
+      <c r="N2" s="17">
         <v>0.35207739999999998</v>
       </c>
       <c r="O2" s="5" t="s">
@@ -1125,7 +1151,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -1134,23 +1160,45 @@
       <c r="C3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
+      <c r="E3" s="6">
+        <v>130</v>
+      </c>
+      <c r="F3" s="8">
+        <v>-9.4095800000000007E-3</v>
+      </c>
+      <c r="G3" s="8">
+        <v>4.8938999999999996E-3</v>
+      </c>
+      <c r="H3" s="8">
+        <v>-1.9227075</v>
+      </c>
+      <c r="I3" s="34">
+        <v>5.6800000000000003E-2</v>
+      </c>
+      <c r="J3" s="8">
+        <v>-1.9001500000000001E-2</v>
+      </c>
+      <c r="K3" s="24">
+        <v>1.8233029999999999E-4</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="8">
+        <v>0.27234940000000002</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -1159,28 +1207,48 @@
       <c r="C4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
+      <c r="E4" s="9">
+        <v>129</v>
+      </c>
+      <c r="F4" s="27">
+        <v>3.8892E-5</v>
+      </c>
+      <c r="G4" s="27">
+        <v>1.7968999999999999E-3</v>
+      </c>
+      <c r="H4" s="19">
+        <v>2.1600000000000001E-2</v>
+      </c>
+      <c r="I4" s="19">
+        <v>0.98280000000000001</v>
+      </c>
+      <c r="J4" s="19">
+        <v>-3.4828810000000002E-3</v>
+      </c>
+      <c r="K4" s="27">
+        <v>3.5606650000000002E-3</v>
+      </c>
+      <c r="L4" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="19">
+        <v>-1.414E-2</v>
+      </c>
+      <c r="N4" s="27">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" s="14"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
+      <c r="A5" s="13"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1189,23 +1257,45 @@
       <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
+      <c r="E6" s="5">
+        <v>798</v>
+      </c>
+      <c r="F6" s="23">
+        <v>1.963E-4</v>
+      </c>
+      <c r="G6" s="23">
+        <v>1.05495E-3</v>
+      </c>
+      <c r="H6" s="17">
+        <v>0.18604599999999999</v>
+      </c>
+      <c r="I6" s="17">
+        <v>0.85250000000000004</v>
+      </c>
+      <c r="J6" s="23">
+        <v>-1.8713950000000001E-3</v>
+      </c>
+      <c r="K6" s="23">
+        <v>2.2639320000000002E-3</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="17">
+        <v>0.35151719999999997</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -1214,23 +1304,45 @@
       <c r="C7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
+      <c r="E7" s="6">
+        <v>130</v>
+      </c>
+      <c r="F7" s="24">
+        <v>7.0621E-3</v>
+      </c>
+      <c r="G7" s="24">
+        <v>4.7571999999999996E-3</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1.4845112</v>
+      </c>
+      <c r="I7" s="8">
+        <v>0.14019999999999999</v>
+      </c>
+      <c r="J7" s="24">
+        <v>-2.2618099999999999E-3</v>
+      </c>
+      <c r="K7" s="8">
+        <v>1.638595E-2</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="8">
+        <v>0.27855829999999998</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -1239,26 +1351,48 @@
       <c r="C8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
+      <c r="E8" s="9">
+        <v>129</v>
+      </c>
+      <c r="F8" s="27">
+        <v>1.6914E-3</v>
+      </c>
+      <c r="G8" s="27">
+        <v>1.3642999999999999E-3</v>
+      </c>
+      <c r="H8" s="19">
+        <v>1.2398</v>
+      </c>
+      <c r="I8" s="19">
+        <v>0.21736</v>
+      </c>
+      <c r="J8" s="27">
+        <v>-9.825286999999999E-4</v>
+      </c>
+      <c r="K8" s="27">
+        <v>4.3653060000000002E-3</v>
+      </c>
+      <c r="L8" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="M8" s="27">
+        <v>-1.92E-3</v>
+      </c>
+      <c r="N8" s="27">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A9" s="15"/>
+      <c r="A9" s="13"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1267,23 +1401,23 @@
       <c r="C10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="30" t="s">
         <v>21</v>
       </c>
       <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
       <c r="O10" s="5"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -1292,23 +1426,23 @@
       <c r="C11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="31" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
       <c r="O11" s="6"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="9" t="s">
@@ -1317,23 +1451,23 @@
       <c r="C12" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="32" t="s">
         <v>21</v>
       </c>
       <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
       <c r="O12" s="9"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -1342,23 +1476,23 @@
       <c r="C14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="35" t="s">
+      <c r="D14" s="30" t="s">
         <v>33</v>
       </c>
       <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
       <c r="O14" s="5"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="6" t="s">
@@ -1367,23 +1501,23 @@
       <c r="C15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="31" t="s">
         <v>33</v>
       </c>
       <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
       <c r="O15" s="6"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="9" t="s">
@@ -1392,23 +1526,24 @@
       <c r="C16" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="37" t="s">
+      <c r="D16" s="32" t="s">
         <v>33</v>
       </c>
       <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
       <c r="O16" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1438,31 +1573,31 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="14" t="s">
         <v>11</v>
       </c>
       <c r="O1" s="3" t="s">
@@ -1470,7 +1605,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1493,7 +1628,7 @@
       <c r="O2" s="5"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -1516,7 +1651,7 @@
       <c r="O3" s="6"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -1539,12 +1674,10 @@
       <c r="O4" s="9"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" s="14"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
+      <c r="A5" s="13"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1567,7 +1700,7 @@
       <c r="O6" s="5"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -1590,7 +1723,7 @@
       <c r="O7" s="6"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -1613,10 +1746,10 @@
       <c r="O8" s="9"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A9" s="15"/>
+      <c r="A9" s="13"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" s="15"/>
+      <c r="A10" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1649,31 +1782,31 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="14" t="s">
         <v>11</v>
       </c>
       <c r="O1" s="3" t="s">
@@ -1681,7 +1814,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1704,7 +1837,7 @@
       <c r="O2" s="5"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -1727,7 +1860,7 @@
       <c r="O3" s="6"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -1750,12 +1883,10 @@
       <c r="O4" s="9"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" s="14"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
+      <c r="A5" s="13"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1778,7 +1909,7 @@
       <c r="O6" s="5"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -1801,7 +1932,7 @@
       <c r="O7" s="6"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -1824,10 +1955,10 @@
       <c r="O8" s="9"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A9" s="15"/>
+      <c r="A9" s="13"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" s="15"/>
+      <c r="A10" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1860,31 +1991,31 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="14" t="s">
         <v>11</v>
       </c>
       <c r="O1" s="3" t="s">
@@ -1892,7 +2023,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1915,7 +2046,7 @@
       <c r="O2" s="5"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -1938,7 +2069,7 @@
       <c r="O3" s="6"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -1961,12 +2092,10 @@
       <c r="O4" s="9"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" s="14"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
+      <c r="A5" s="13"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1989,7 +2118,7 @@
       <c r="O6" s="5"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -2012,7 +2141,7 @@
       <c r="O7" s="6"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -2035,10 +2164,10 @@
       <c r="O8" s="9"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A9" s="15"/>
+      <c r="A9" s="13"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" s="15"/>
+      <c r="A10" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2071,31 +2200,31 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="14" t="s">
         <v>11</v>
       </c>
       <c r="O1" s="3" t="s">
@@ -2103,7 +2232,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2126,7 +2255,7 @@
       <c r="O2" s="5"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -2149,7 +2278,7 @@
       <c r="O3" s="6"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -2172,12 +2301,10 @@
       <c r="O4" s="9"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" s="14"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
+      <c r="A5" s="13"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -2200,7 +2327,7 @@
       <c r="O6" s="5"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -2223,7 +2350,7 @@
       <c r="O7" s="6"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -2246,10 +2373,10 @@
       <c r="O8" s="9"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A9" s="15"/>
+      <c r="A9" s="13"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" s="15"/>
+      <c r="A10" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2282,31 +2409,31 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="14" t="s">
         <v>11</v>
       </c>
       <c r="O1" s="3" t="s">
@@ -2314,7 +2441,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2337,7 +2464,7 @@
       <c r="O2" s="5"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -2360,7 +2487,7 @@
       <c r="O3" s="6"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -2383,15 +2510,13 @@
       <c r="O4" s="9"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" s="14"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
+      <c r="A5" s="13"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" s="15"/>
+      <c r="A6" s="13"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" s="15"/>
+      <c r="A7" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Done with Diet Traits and Life History Traits results!
</commit_message>
<xml_diff>
--- a/Results/Update Coastal_RESULTS.xlsx
+++ b/Results/Update Coastal_RESULTS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/emgarris_calpoly_edu/Documents/R_Projects/CoastalBirdsUPDATE/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="621" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D72D7546-D26E-4E7E-857A-7D7696B0FE0B}"/>
+  <xr:revisionPtr revIDLastSave="946" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{758E40F0-3150-4B9F-82AF-E042198038E6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sensory" sheetId="4" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="66">
   <si>
     <t>Index used</t>
   </si>
@@ -168,6 +168,78 @@
   </si>
   <si>
     <t xml:space="preserve">0.01373	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/ </t>
+  </si>
+  <si>
+    <t>low collinearity, q-q plot falls off of line at ends</t>
+  </si>
+  <si>
+    <t>normal q-q plot good and binomial distributions look normal</t>
+  </si>
+  <si>
+    <t>Diet</t>
+  </si>
+  <si>
+    <t>Life History</t>
+  </si>
+  <si>
+    <t>brood value</t>
+  </si>
+  <si>
+    <t>clutch size</t>
+  </si>
+  <si>
+    <t>longevity</t>
+  </si>
+  <si>
+    <t>developmental mode</t>
+  </si>
+  <si>
+    <t>low collinearity, q-q plot good, falls off line at the ends</t>
+  </si>
+  <si>
+    <t>low collinearity, q-q line not very fit… low linearity of residuals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.01137	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.02075	</t>
+  </si>
+  <si>
+    <t>Nesting Strategy (Open/Enclosed)</t>
+  </si>
+  <si>
+    <t>Nesting Site (High)</t>
+  </si>
+  <si>
+    <t>Nesting Site (Low)</t>
+  </si>
+  <si>
+    <t>Nest Safety</t>
+  </si>
+  <si>
+    <t>Dichromatism (Brightness)</t>
+  </si>
+  <si>
+    <t>Dichromatism (Hue)</t>
+  </si>
+  <si>
+    <t>Sex Selection Intensity (Male)</t>
+  </si>
+  <si>
+    <t>Sex Selection Intensity (Female)</t>
+  </si>
+  <si>
+    <t>Territoriality</t>
+  </si>
+  <si>
+    <t>Cooperative Breeding</t>
+  </si>
+  <si>
+    <t>log(Body Mass)</t>
   </si>
 </sst>
 </file>
@@ -178,7 +250,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +286,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -322,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -388,6 +468,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -674,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F82655-FE3A-4F4B-B446-2D913CF0CC8B}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1039,19 +1123,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C8F29B3-A633-40B8-A222-FC489EFBC75D}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="18.26953125" style="33" customWidth="1"/>
-    <col min="6" max="6" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.7265625" style="4"/>
-    <col min="10" max="10" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7265625" style="4"/>
+    <col min="6" max="6" width="9.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7265625" style="4"/>
+    <col min="10" max="10" width="9.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.08984375" style="4" bestFit="1" customWidth="1"/>
   </cols>
@@ -1111,7 +1197,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="D2" s="30" t="s">
         <v>31</v>
@@ -1158,7 +1244,7 @@
         <v>18</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="D3" s="31" t="s">
         <v>31</v>
@@ -1205,7 +1291,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="D4" s="32" t="s">
         <v>31</v>
@@ -1255,7 +1341,7 @@
         <v>18</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="D6" s="30" t="s">
         <v>32</v>
@@ -1302,7 +1388,7 @@
         <v>18</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>32</v>
@@ -1319,7 +1405,7 @@
       <c r="H7" s="8">
         <v>1.4845112</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="36">
         <v>0.14019999999999999</v>
       </c>
       <c r="J7" s="24">
@@ -1349,7 +1435,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="D8" s="32" t="s">
         <v>32</v>
@@ -1399,22 +1485,44 @@
         <v>18</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="D10" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="5"/>
+      <c r="E10" s="5">
+        <v>798</v>
+      </c>
+      <c r="F10" s="23">
+        <v>1.7090000000000001E-4</v>
+      </c>
+      <c r="G10" s="23">
+        <v>1.11808E-3</v>
+      </c>
+      <c r="H10" s="17">
+        <v>0.15283099999999999</v>
+      </c>
+      <c r="I10" s="17">
+        <v>0.87860000000000005</v>
+      </c>
+      <c r="J10" s="23">
+        <v>-2.020516E-3</v>
+      </c>
+      <c r="K10" s="23">
+        <v>2.3622690000000002E-3</v>
+      </c>
+      <c r="L10" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="M10" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="N10" s="17">
+        <v>0.35064200000000001</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
@@ -1424,22 +1532,45 @@
         <v>18</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="6"/>
+      <c r="E11" s="6">
+        <v>130</v>
+      </c>
+      <c r="F11" s="24">
+        <v>1.6699999999999999E-5</v>
+      </c>
+      <c r="G11" s="24">
+        <v>5.3559000000000002E-3</v>
+      </c>
+      <c r="H11" s="24">
+        <v>3.1189999999999998E-3</v>
+      </c>
+      <c r="I11" s="8">
+        <v>0.99750000000000005</v>
+      </c>
+      <c r="J11" s="24">
+        <f>--0.01048071</f>
+        <v>1.0480710000000001E-2</v>
+      </c>
+      <c r="K11" s="24">
+        <v>1.051412E-2</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N11" s="8">
+        <v>0.29122520000000002</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
@@ -1449,22 +1580,44 @@
         <v>13</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="D12" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="9"/>
+      <c r="E12" s="9">
+        <v>129</v>
+      </c>
+      <c r="F12" s="27">
+        <v>-2.1262999999999998E-3</v>
+      </c>
+      <c r="G12" s="27">
+        <v>-2.1262999999999998E-3</v>
+      </c>
+      <c r="H12" s="19">
+        <v>-1.4541999999999999</v>
+      </c>
+      <c r="I12" s="35">
+        <v>0.1484</v>
+      </c>
+      <c r="J12" s="27">
+        <v>-4.9921100000000001E-3</v>
+      </c>
+      <c r="K12" s="27">
+        <v>7.3954960000000003E-4</v>
+      </c>
+      <c r="L12" s="19">
+        <v>1.8180000000000002E-2</v>
+      </c>
+      <c r="M12" s="27">
+        <v>2.5969999999999999E-3</v>
+      </c>
+      <c r="N12" s="27">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
@@ -1474,22 +1627,44 @@
         <v>18</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="D14" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="5"/>
+      <c r="E14" s="5">
+        <v>798</v>
+      </c>
+      <c r="F14" s="23">
+        <v>9.3809999999999998E-4</v>
+      </c>
+      <c r="G14" s="23">
+        <v>2.2045300000000001E-3</v>
+      </c>
+      <c r="H14" s="17">
+        <v>0.42555199999999999</v>
+      </c>
+      <c r="I14" s="17">
+        <v>0.67049999999999998</v>
+      </c>
+      <c r="J14" s="23">
+        <v>-3.3826519999999999E-3</v>
+      </c>
+      <c r="K14" s="23">
+        <v>5.2589309999999997E-3</v>
+      </c>
+      <c r="L14" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="M14" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="N14" s="17">
+        <v>0.34664660000000003</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
@@ -1499,22 +1674,44 @@
         <v>18</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="6"/>
+      <c r="E15" s="6">
+        <v>130</v>
+      </c>
+      <c r="F15" s="8">
+        <v>2.0850299999999999E-2</v>
+      </c>
+      <c r="G15" s="8">
+        <v>1.6558199999999999E-2</v>
+      </c>
+      <c r="H15" s="8">
+        <v>1.2592179999999999</v>
+      </c>
+      <c r="I15" s="8">
+        <v>0.21029999999999999</v>
+      </c>
+      <c r="J15" s="8">
+        <v>-1.160306E-2</v>
+      </c>
+      <c r="K15" s="8">
+        <v>5.3303730000000001E-2</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N15" s="8">
+        <v>0.26359830000000001</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
@@ -1524,22 +1721,44 @@
         <v>13</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="D16" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
-      <c r="O16" s="9"/>
+      <c r="E16" s="9">
+        <v>129</v>
+      </c>
+      <c r="F16" s="27">
+        <v>1.6590000000000001E-3</v>
+      </c>
+      <c r="G16" s="27">
+        <v>4.9274000000000002E-3</v>
+      </c>
+      <c r="H16" s="19">
+        <v>0.3367</v>
+      </c>
+      <c r="I16" s="19">
+        <v>0.73692000000000002</v>
+      </c>
+      <c r="J16" s="27">
+        <v>-7.9984940000000001E-3</v>
+      </c>
+      <c r="K16" s="27">
+        <v>1.1316430000000001E-2</v>
+      </c>
+      <c r="L16" s="27">
+        <v>2.601E-3</v>
+      </c>
+      <c r="M16" s="19">
+        <v>-1.323E-2</v>
+      </c>
+      <c r="N16" s="27">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1549,10 +1768,655 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8E188F-C842-439D-93EC-074F9278CAC0}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K20" sqref="K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="11.81640625" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" customWidth="1"/>
+    <col min="6" max="6" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="8.7265625" style="4"/>
+    <col min="11" max="11" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="5">
+        <v>480</v>
+      </c>
+      <c r="F2" s="17">
+        <v>-0.16023960000000001</v>
+      </c>
+      <c r="G2" s="17">
+        <v>7.7241359999999995E-2</v>
+      </c>
+      <c r="H2" s="17">
+        <v>-2.0745309999999999</v>
+      </c>
+      <c r="I2" s="37">
+        <v>3.8600000000000002E-2</v>
+      </c>
+      <c r="J2" s="17">
+        <v>-0.31162990000000002</v>
+      </c>
+      <c r="K2" s="23">
+        <v>-8.8493200000000008E-3</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="17">
+        <v>0.41643530000000001</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="6">
+        <v>121</v>
+      </c>
+      <c r="F3" s="8">
+        <v>-0.46318239999999999</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0.43608950000000002</v>
+      </c>
+      <c r="H3" s="8">
+        <v>-1.0621267999999999</v>
+      </c>
+      <c r="I3" s="8">
+        <v>0.2903</v>
+      </c>
+      <c r="J3" s="8">
+        <v>-1.3179021</v>
+      </c>
+      <c r="K3" s="8">
+        <v>0.39153739999999998</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="8">
+        <v>0.25423780000000001</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="9">
+        <v>102</v>
+      </c>
+      <c r="F4" s="19">
+        <v>-6.4863000000000004E-2</v>
+      </c>
+      <c r="G4" s="19">
+        <v>0.17649599999999999</v>
+      </c>
+      <c r="H4" s="19">
+        <v>-0.36749999999999999</v>
+      </c>
+      <c r="I4" s="19">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="J4" s="19">
+        <v>-0.41078854999999997</v>
+      </c>
+      <c r="K4" s="19">
+        <v>0.28106309000000002</v>
+      </c>
+      <c r="L4" s="27">
+        <v>5.5279999999999999E-3</v>
+      </c>
+      <c r="M4" s="19">
+        <v>-1.456E-2</v>
+      </c>
+      <c r="N4" s="19">
+        <v>6.9250500000000006E-2</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" s="13"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="5">
+        <v>738</v>
+      </c>
+      <c r="F6" s="17">
+        <v>5.0438900000000002E-2</v>
+      </c>
+      <c r="G6" s="17">
+        <v>1.463736E-2</v>
+      </c>
+      <c r="H6" s="17">
+        <v>3.4458980000000001</v>
+      </c>
+      <c r="I6" s="37">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="J6" s="17">
+        <v>2.1750160000000001E-2</v>
+      </c>
+      <c r="K6" s="17">
+        <v>7.9127550000000005E-2</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="17">
+        <v>0.31013429999999997</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="6">
+        <v>126</v>
+      </c>
+      <c r="F7" s="8">
+        <v>7.2733599999999995E-2</v>
+      </c>
+      <c r="G7" s="8">
+        <v>8.0693600000000004E-2</v>
+      </c>
+      <c r="H7" s="8">
+        <v>0.90135600000000005</v>
+      </c>
+      <c r="I7" s="8">
+        <v>0.36919999999999997</v>
+      </c>
+      <c r="J7" s="8">
+        <v>-8.542284E-2</v>
+      </c>
+      <c r="K7" s="8">
+        <v>0.23089009999999999</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="8">
+        <v>0.37893369999999998</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="9">
+        <v>122</v>
+      </c>
+      <c r="F8" s="19">
+        <v>-1.9120999999999999E-2</v>
+      </c>
+      <c r="G8" s="19">
+        <v>1.8939999999999999E-2</v>
+      </c>
+      <c r="H8" s="19">
+        <v>-1.0096000000000001</v>
+      </c>
+      <c r="I8" s="19">
+        <v>0.31474999999999997</v>
+      </c>
+      <c r="J8" s="19">
+        <v>-5.624349E-2</v>
+      </c>
+      <c r="K8" s="19">
+        <v>1.800086E-2</v>
+      </c>
+      <c r="L8" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="M8" s="27">
+        <v>-5.2469999999999999E-3</v>
+      </c>
+      <c r="N8" s="27">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" s="13"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="5">
+        <v>796</v>
+      </c>
+      <c r="F10" s="23">
+        <v>-7.5303999999999996E-3</v>
+      </c>
+      <c r="G10" s="23">
+        <v>5.7165000000000002E-3</v>
+      </c>
+      <c r="H10" s="17">
+        <v>-1.3172999999999999</v>
+      </c>
+      <c r="I10" s="38">
+        <v>0.18809999999999999</v>
+      </c>
+      <c r="J10" s="17">
+        <v>-1.8734489999999999E-2</v>
+      </c>
+      <c r="K10" s="23">
+        <v>3.6737900000000001E-3</v>
+      </c>
+      <c r="L10" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" s="17">
+        <v>0.30335590000000001</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="6">
+        <v>130</v>
+      </c>
+      <c r="F11" s="8">
+        <v>-2.88133E-2</v>
+      </c>
+      <c r="G11" s="8">
+        <v>3.3878800000000001E-2</v>
+      </c>
+      <c r="H11" s="8">
+        <v>-0.85048360000000001</v>
+      </c>
+      <c r="I11" s="8">
+        <v>0.3967</v>
+      </c>
+      <c r="J11" s="8">
+        <v>-9.5214480000000004E-2</v>
+      </c>
+      <c r="K11" s="8">
+        <v>3.7587820000000001E-2</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N11" s="8">
+        <v>0.29893370000000002</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="9">
+        <v>129</v>
+      </c>
+      <c r="F12" s="27">
+        <v>-2.4012999999999999E-3</v>
+      </c>
+      <c r="G12" s="19">
+        <v>1.1044699999999999E-2</v>
+      </c>
+      <c r="H12" s="19">
+        <v>-0.21740000000000001</v>
+      </c>
+      <c r="I12" s="19">
+        <v>0.82823000000000002</v>
+      </c>
+      <c r="J12" s="19">
+        <v>-2.4048594999999999E-2</v>
+      </c>
+      <c r="K12" s="19">
+        <v>1.9245950000000001E-2</v>
+      </c>
+      <c r="L12" s="27">
+        <v>2.078E-3</v>
+      </c>
+      <c r="M12" s="27">
+        <v>-1.376E-2</v>
+      </c>
+      <c r="N12" s="27">
+        <v>1.081113E-7</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="5">
+        <v>766</v>
+      </c>
+      <c r="F14" s="17">
+        <v>-3.5994699999999998E-2</v>
+      </c>
+      <c r="G14" s="17">
+        <v>0.14913986000000001</v>
+      </c>
+      <c r="H14" s="17">
+        <v>-0.24134900000000001</v>
+      </c>
+      <c r="I14" s="17">
+        <v>0.80930000000000002</v>
+      </c>
+      <c r="J14" s="17">
+        <v>-0.32830348999999998</v>
+      </c>
+      <c r="K14" s="17">
+        <v>0.25631401199999998</v>
+      </c>
+      <c r="L14" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="M14" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14" s="17">
+        <v>0.38511570000000001</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="6">
+        <v>127</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.87056990000000001</v>
+      </c>
+      <c r="G15" s="8">
+        <v>0.40333200000000002</v>
+      </c>
+      <c r="H15" s="8">
+        <v>2.1584449999999999</v>
+      </c>
+      <c r="I15" s="34">
+        <v>3.2800000000000003E-2</v>
+      </c>
+      <c r="J15" s="8">
+        <v>8.0053689999999997E-2</v>
+      </c>
+      <c r="K15" s="8">
+        <v>1.6610862</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N15" s="8">
+        <v>0.25619589999999998</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="9">
+        <v>129</v>
+      </c>
+      <c r="F16" s="19">
+        <v>0.16307099999999999</v>
+      </c>
+      <c r="G16" s="19">
+        <v>0.104157</v>
+      </c>
+      <c r="H16" s="19">
+        <v>1.5656000000000001</v>
+      </c>
+      <c r="I16" s="35">
+        <v>0.11990000000000001</v>
+      </c>
+      <c r="J16" s="19">
+        <v>-4.1072039999999997E-2</v>
+      </c>
+      <c r="K16" s="19">
+        <v>0.36721503</v>
+      </c>
+      <c r="L16" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="M16" s="19">
+        <v>5.2100000000000002E-3</v>
+      </c>
+      <c r="N16" s="19">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA225CA-067B-4F77-85FD-EE40FC6CFFCC}">
+  <dimension ref="A1:O16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1614,7 +2478,9 @@
       <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -1637,7 +2503,9 @@
       <c r="C3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>57</v>
+      </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -1660,7 +2528,9 @@
       <c r="C4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="9"/>
+      <c r="D4" s="9" t="s">
+        <v>57</v>
+      </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
@@ -1686,7 +2556,9 @@
       <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -1709,7 +2581,9 @@
       <c r="C7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -1732,7 +2606,9 @@
       <c r="C8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="9"/>
+      <c r="D8" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
@@ -1749,22 +2625,173 @@
       <c r="A9" s="13"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" s="13"/>
+      <c r="A10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA225CA-067B-4F77-85FD-EE40FC6CFFCC}">
-  <dimension ref="A1:O10"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44B5211-D37C-46F5-A2CD-0BEBDDA2FFCE}">
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="30" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
@@ -1823,7 +2850,9 @@
       <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -1846,7 +2875,9 @@
       <c r="C3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -1869,7 +2900,9 @@
       <c r="C4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="9"/>
+      <c r="D4" s="9" t="s">
+        <v>59</v>
+      </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
@@ -1895,7 +2928,9 @@
       <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -1918,7 +2953,9 @@
       <c r="C7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -1941,7 +2978,9 @@
       <c r="C8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="9"/>
+      <c r="D8" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
@@ -1958,19 +2997,166 @@
       <c r="A9" s="13"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" s="13"/>
+      <c r="A10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44B5211-D37C-46F5-A2CD-0BEBDDA2FFCE}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D19BA0CD-B3A4-4C64-A7BB-E12896AEF890}">
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2032,7 +3218,9 @@
       <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -2055,7 +3243,9 @@
       <c r="C3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -2078,7 +3268,9 @@
       <c r="C4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="9"/>
+      <c r="D4" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
@@ -2104,7 +3296,9 @@
       <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -2127,7 +3321,9 @@
       <c r="C7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -2150,7 +3346,9 @@
       <c r="C8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="9"/>
+      <c r="D8" s="9" t="s">
+        <v>64</v>
+      </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
@@ -2174,12 +3372,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D19BA0CD-B3A4-4C64-A7BB-E12896AEF890}">
-  <dimension ref="A1:O10"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0232423-D4EE-4B15-B8EC-2DF31E8640A1}">
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2241,7 +3439,9 @@
       <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>65</v>
+      </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -2264,7 +3464,9 @@
       <c r="C3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -2287,7 +3489,9 @@
       <c r="C4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="9"/>
+      <c r="D4" s="9" t="s">
+        <v>65</v>
+      </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
@@ -2304,215 +3508,6 @@
       <c r="A5" s="13"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A9" s="13"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" s="13"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0232423-D4EE-4B15-B8EC-2DF31E8640A1}">
-  <dimension ref="A1:O7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:15" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" s="13"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="13"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
half of nesting trait results committ
</commit_message>
<xml_diff>
--- a/Results/Update Coastal_RESULTS.xlsx
+++ b/Results/Update Coastal_RESULTS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/emgarris_calpoly_edu/Documents/R_Projects/CoastalBirdsUPDATE/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="946" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{758E40F0-3150-4B9F-82AF-E042198038E6}"/>
+  <xr:revisionPtr revIDLastSave="1024" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B0E8CC1-31BD-4512-94C1-B16FDA47FB14}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4670" yWindow="1170" windowWidth="14400" windowHeight="8170" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sensory" sheetId="4" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="71">
   <si>
     <t>Index used</t>
   </si>
@@ -240,6 +240,21 @@
   </si>
   <si>
     <t>log(Body Mass)</t>
+  </si>
+  <si>
+    <t>low collinearity, good normality of residuals, q-q line falls off on ends</t>
+  </si>
+  <si>
+    <t>low collinearity, q-q line falls off on ends</t>
+  </si>
+  <si>
+    <t>normal q-q and normality of residuals shows some datapoints well off line/bell curve</t>
+  </si>
+  <si>
+    <t>low collinearity, q-q line is ok, but falls off at ends</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.01791	</t>
   </si>
 </sst>
 </file>
@@ -402,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -472,6 +487,8 @@
     <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F82655-FE3A-4F4B-B446-2D913CF0CC8B}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2414,14 +2431,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA225CA-067B-4F77-85FD-EE40FC6CFFCC}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
+      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="30.6328125" customWidth="1"/>
+    <col min="6" max="10" width="8.7265625" style="4"/>
+    <col min="11" max="11" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2481,17 +2503,39 @@
       <c r="D2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
+      <c r="E2" s="5">
+        <v>796</v>
+      </c>
+      <c r="F2" s="17">
+        <v>-0.1150249</v>
+      </c>
+      <c r="G2" s="17">
+        <v>5.501176E-2</v>
+      </c>
+      <c r="H2" s="17">
+        <v>-2.0909149999999999</v>
+      </c>
+      <c r="I2" s="37">
+        <v>3.6900000000000002E-2</v>
+      </c>
+      <c r="J2" s="17">
+        <v>-0.22284593999999999</v>
+      </c>
+      <c r="K2" s="23">
+        <v>-7.2038249999999996E-3</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="5">
+        <v>0.31788480000000002</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
@@ -2506,17 +2550,39 @@
       <c r="D3" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
+      <c r="E3" s="6">
+        <v>130</v>
+      </c>
+      <c r="F3" s="8">
+        <v>-0.51787050000000001</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0.293076</v>
+      </c>
+      <c r="H3" s="8">
+        <v>-1.767018</v>
+      </c>
+      <c r="I3" s="34">
+        <v>7.9600000000000004E-2</v>
+      </c>
+      <c r="J3" s="8">
+        <v>-1.0922888230000001</v>
+      </c>
+      <c r="K3" s="8">
+        <v>5.6547790000000001E-2</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="6">
+        <v>0.1613368</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
@@ -2531,17 +2597,39 @@
       <c r="D4" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
+      <c r="E4" s="9">
+        <v>129</v>
+      </c>
+      <c r="F4" s="19">
+        <v>-0.247531</v>
+      </c>
+      <c r="G4" s="19">
+        <v>0.17519100000000001</v>
+      </c>
+      <c r="H4" s="19">
+        <v>-1.4129</v>
+      </c>
+      <c r="I4" s="40">
+        <v>0.16028999999999999</v>
+      </c>
+      <c r="J4" s="19">
+        <v>-0.59089959999999997</v>
+      </c>
+      <c r="K4" s="19">
+        <v>9.5837240000000004E-2</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="M4" s="9">
+        <v>1.4090000000000001E-3</v>
+      </c>
+      <c r="N4" s="39">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="13"/>
@@ -2560,14 +2648,18 @@
         <v>56</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
     </row>
@@ -2585,14 +2677,18 @@
         <v>56</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
     </row>
@@ -2610,12 +2706,12 @@
         <v>56</v>
       </c>
       <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
@@ -2637,17 +2733,39 @@
       <c r="D10" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
+      <c r="E10" s="5">
+        <v>733</v>
+      </c>
+      <c r="F10" s="17">
+        <v>3.3735099999999997E-2</v>
+      </c>
+      <c r="G10" s="17">
+        <v>7.7621560000000006E-2</v>
+      </c>
+      <c r="H10" s="17">
+        <v>0.43460900000000002</v>
+      </c>
+      <c r="I10" s="17">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="J10" s="17">
+        <v>-0.11840041</v>
+      </c>
+      <c r="K10" s="17">
+        <v>0.18587053000000001</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" s="17">
+        <v>0.37230829999999998</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
@@ -2662,17 +2780,39 @@
       <c r="D11" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
+      <c r="E11" s="6">
+        <v>117</v>
+      </c>
+      <c r="F11" s="8">
+        <v>-0.21963659999999999</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0.49134080000000002</v>
+      </c>
+      <c r="H11" s="8">
+        <v>-0.44701469999999999</v>
+      </c>
+      <c r="I11" s="8">
+        <v>0.65569999999999995</v>
+      </c>
+      <c r="J11" s="8">
+        <v>-1.1826467700000001</v>
+      </c>
+      <c r="K11" s="8">
+        <v>0.74337370000000003</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N11" s="8">
+        <v>0.3196425</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
@@ -2687,17 +2827,39 @@
       <c r="D12" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
+      <c r="E12" s="9">
+        <v>122</v>
+      </c>
+      <c r="F12" s="19">
+        <v>-0.247531</v>
+      </c>
+      <c r="G12" s="19">
+        <v>0.17519100000000001</v>
+      </c>
+      <c r="H12" s="19">
+        <v>-1.4129</v>
+      </c>
+      <c r="I12" s="35">
+        <v>0.16028999999999999</v>
+      </c>
+      <c r="J12" s="19">
+        <v>-0.59089959999999997</v>
+      </c>
+      <c r="K12" s="19">
+        <v>9.5837240000000004E-2</v>
+      </c>
+      <c r="L12" s="9">
+        <v>1.7909999999999999E-2</v>
+      </c>
+      <c r="M12" s="9">
+        <v>1.4090000000000001E-3</v>
+      </c>
+      <c r="N12" s="39">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
@@ -2713,14 +2875,18 @@
         <v>58</v>
       </c>
       <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
@@ -2738,14 +2904,18 @@
         <v>58</v>
       </c>
       <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
     </row>
@@ -2763,12 +2933,12 @@
         <v>58</v>
       </c>
       <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
@@ -2776,6 +2946,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
done with results!!! need to omit models with binomial character traits that do not have n>10 for each 0 and 1
</commit_message>
<xml_diff>
--- a/Results/Update Coastal_RESULTS.xlsx
+++ b/Results/Update Coastal_RESULTS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/emgarris_calpoly_edu/Documents/R_Projects/CoastalBirdsUPDATE/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1024" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B0E8CC1-31BD-4512-94C1-B16FDA47FB14}"/>
+  <xr:revisionPtr revIDLastSave="1335" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43CA74E2-D44C-4F8F-92CB-28EC93D90D02}"/>
   <bookViews>
-    <workbookView xWindow="4670" yWindow="1170" windowWidth="14400" windowHeight="8170" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4670" yWindow="1170" windowWidth="14400" windowHeight="8170" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sensory" sheetId="4" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="101">
   <si>
     <t>Index used</t>
   </si>
@@ -255,6 +255,96 @@
   </si>
   <si>
     <t xml:space="preserve">0.01791	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">normal q-q okay for binomial, distributions not strictly normal but look okay </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.03792	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">low collinearity, good normality of residuals, q-q line trails off on ends but good otherwise </t>
+  </si>
+  <si>
+    <t xml:space="preserve">low collinearity, seems to be one residual outlier? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.03299	</t>
+  </si>
+  <si>
+    <t>low collinearity, low q-q looks good, potentially a few outliers on ends</t>
+  </si>
+  <si>
+    <t xml:space="preserve">error with corpagel = 0.5, F --&gt; error with corpagel = 0.1, T : q-q okay, not the best normality of residuals (smaller sample size) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0547	</t>
+  </si>
+  <si>
+    <t>binomial distributions look okay, q-q plot looks okay for smaller sample size</t>
+  </si>
+  <si>
+    <t>low collinearity, q-q line looks great with just a few species trailing off</t>
+  </si>
+  <si>
+    <t>low collinearity, q-q okay, not the best normality of residuals (smaller sample size?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.06742	</t>
+  </si>
+  <si>
+    <t>binomial distributions look okay, q-q plot just alright..</t>
+  </si>
+  <si>
+    <t xml:space="preserve">low collinearity, q-q okay </t>
+  </si>
+  <si>
+    <t>q-q plot and residual histograms look good!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.005452	</t>
+  </si>
+  <si>
+    <t>low collinearity, q-q okay but trails off at ends</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.007978	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for binomial distribution, q-q and histograms look okay </t>
+  </si>
+  <si>
+    <t xml:space="preserve">low collinearity, good normality of residuals, q-q plot looks good - trails off line at ends </t>
+  </si>
+  <si>
+    <t>low collinearity, q-q plot looks good but trails off at ends</t>
+  </si>
+  <si>
+    <t>q-q plot looks good, histogram of residuals fairly normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.01048	</t>
+  </si>
+  <si>
+    <t>low collinearity, histogram of residuals a little skewed right</t>
+  </si>
+  <si>
+    <t>definitely some outliers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0574	</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> q-q plot looks good but trails off on ends</t>
+  </si>
+  <si>
+    <t>q-q plot looks good, trails off more on left end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001703	</t>
+  </si>
+  <si>
+    <t>q-q plot looks good for binomial distribution</t>
   </si>
 </sst>
 </file>
@@ -417,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -489,6 +579,7 @@
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -775,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F82655-FE3A-4F4B-B446-2D913CF0CC8B}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2431,15 +2522,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA225CA-067B-4F77-85FD-EE40FC6CFFCC}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="30.6328125" customWidth="1"/>
-    <col min="6" max="10" width="8.7265625" style="4"/>
+    <col min="6" max="8" width="8.7265625" style="4"/>
+    <col min="9" max="9" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7265625" style="4"/>
     <col min="11" max="11" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2647,21 +2740,39 @@
       <c r="D6" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
+      <c r="E6" s="5">
+        <v>796</v>
+      </c>
+      <c r="F6" s="17">
+        <v>0.17676629999999999</v>
+      </c>
+      <c r="G6" s="17">
+        <v>5.066615E-2</v>
+      </c>
+      <c r="H6" s="17">
+        <v>3.4888439999999998</v>
+      </c>
+      <c r="I6" s="41">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="J6" s="17">
+        <v>7.7462470000000005E-2</v>
+      </c>
+      <c r="K6" s="17">
+        <v>0.27607010999999998</v>
+      </c>
       <c r="L6" s="5" t="s">
         <v>27</v>
       </c>
       <c r="M6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
+      <c r="N6" s="5">
+        <v>0.32124799999999998</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
@@ -2676,21 +2787,39 @@
       <c r="D7" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
+      <c r="E7" s="6">
+        <v>130</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.37727919999999998</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0.26005499999999998</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1.4507669999999999</v>
+      </c>
+      <c r="I7" s="36">
+        <v>0.14929999999999999</v>
+      </c>
+      <c r="J7" s="8">
+        <v>-0.13241919999999999</v>
+      </c>
+      <c r="K7" s="8">
+        <v>0.88697769999999998</v>
+      </c>
       <c r="L7" s="6" t="s">
         <v>27</v>
       </c>
       <c r="M7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
+      <c r="N7" s="6">
+        <v>0.19552069999999999</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
@@ -2705,17 +2834,39 @@
       <c r="D8" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
+      <c r="E8" s="9">
+        <v>129</v>
+      </c>
+      <c r="F8" s="19">
+        <v>0.18750500000000001</v>
+      </c>
+      <c r="G8" s="19">
+        <v>8.6096000000000006E-2</v>
+      </c>
+      <c r="H8" s="19">
+        <v>2.1779000000000002</v>
+      </c>
+      <c r="I8" s="40">
+        <v>3.1280000000000002E-2</v>
+      </c>
+      <c r="J8" s="19">
+        <v>1.8760120000000002E-2</v>
+      </c>
+      <c r="K8" s="19">
+        <v>0.3562496</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="M8" s="9">
+        <v>2.265E-2</v>
+      </c>
+      <c r="N8" s="39">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="13"/>
@@ -2874,21 +3025,39 @@
       <c r="D14" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
+      <c r="E14" s="5">
+        <v>766</v>
+      </c>
+      <c r="F14" s="17">
+        <v>1.28252E-2</v>
+      </c>
+      <c r="G14" s="17">
+        <v>2.7534159999999998E-2</v>
+      </c>
+      <c r="H14" s="17">
+        <v>0.46579300000000001</v>
+      </c>
+      <c r="I14" s="17">
+        <v>0.64149999999999996</v>
+      </c>
+      <c r="J14" s="17">
+        <v>-4.1140749999999997E-2</v>
+      </c>
+      <c r="K14" s="17">
+        <v>6.6791181000000005E-2</v>
+      </c>
       <c r="L14" s="5" t="s">
         <v>27</v>
       </c>
       <c r="M14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
+      <c r="N14" s="5">
+        <v>0.39305909999999999</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
@@ -2903,21 +3072,39 @@
       <c r="D15" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
+      <c r="E15" s="6">
+        <v>127</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.17732239999999999</v>
+      </c>
+      <c r="G15" s="8">
+        <v>0.14088790000000001</v>
+      </c>
+      <c r="H15" s="8">
+        <v>1.2586059999999999</v>
+      </c>
+      <c r="I15" s="8">
+        <v>0.21049999999999999</v>
+      </c>
+      <c r="J15" s="8">
+        <v>-9.8812860000000002E-2</v>
+      </c>
+      <c r="K15" s="8">
+        <v>0.45345760000000002</v>
+      </c>
       <c r="L15" s="6" t="s">
         <v>27</v>
       </c>
       <c r="M15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
+      <c r="N15" s="6">
+        <v>0.3511283</v>
+      </c>
+      <c r="O15" s="11" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
@@ -2932,17 +3119,39 @@
       <c r="D16" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
+      <c r="E16" s="9">
+        <v>129</v>
+      </c>
+      <c r="F16" s="19">
+        <v>0.1242379</v>
+      </c>
+      <c r="G16" s="19">
+        <v>6.1530500000000002E-2</v>
+      </c>
+      <c r="H16" s="19">
+        <v>2.0190999999999999</v>
+      </c>
+      <c r="I16" s="40">
+        <v>4.5600000000000002E-2</v>
+      </c>
+      <c r="J16" s="19">
+        <v>3.6402560000000001E-3</v>
+      </c>
+      <c r="K16" s="19">
+        <v>0.24483557</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="M16" s="9">
+        <v>1.7639999999999999E-2</v>
+      </c>
+      <c r="N16" s="39">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2954,9 +3163,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44B5211-D37C-46F5-A2CD-0BEBDDA2FFCE}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2964,7 +3173,7 @@
     <col min="4" max="4" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3024,17 +3233,39 @@
       <c r="D2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
+      <c r="E2" s="5">
+        <v>201</v>
+      </c>
+      <c r="F2" s="5">
+        <v>3.2897999999999998E-3</v>
+      </c>
+      <c r="G2" s="5">
+        <v>4.1466999999999997E-3</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0.79335800000000001</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0.42849999999999999</v>
+      </c>
+      <c r="J2" s="5">
+        <v>-4.8375750000000002E-3</v>
+      </c>
+      <c r="K2" s="5">
+        <v>1.141722E-2</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="5">
+        <v>0.79097019999999996</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
@@ -3049,17 +3280,39 @@
       <c r="D3" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
+      <c r="E3" s="6">
+        <v>67</v>
+      </c>
+      <c r="F3" s="6">
+        <v>2.9464000000000001E-3</v>
+      </c>
+      <c r="G3" s="6">
+        <v>1.8641999999999999E-2</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0.15804950000000001</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0.87490000000000001</v>
+      </c>
+      <c r="J3" s="6">
+        <v>-3.3591309999999999E-2</v>
+      </c>
+      <c r="K3" s="6">
+        <v>3.9484030000000003E-2</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
@@ -3074,17 +3327,39 @@
       <c r="D4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
+      <c r="E4" s="9">
+        <v>61</v>
+      </c>
+      <c r="F4" s="9">
+        <v>-8.1607999999999993E-3</v>
+      </c>
+      <c r="G4" s="9">
+        <v>1.2829399999999999E-2</v>
+      </c>
+      <c r="H4" s="9">
+        <v>-0.6361</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0.5272</v>
+      </c>
+      <c r="J4" s="9">
+        <v>-3.3306049999999997E-2</v>
+      </c>
+      <c r="K4" s="9">
+        <v>1.6984369999999999E-2</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="M4" s="9">
+        <v>2.2100000000000002E-2</v>
+      </c>
+      <c r="N4" s="9">
+        <v>0.22558120000000001</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="13"/>
@@ -3102,17 +3377,39 @@
       <c r="D6" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
+      <c r="E6" s="5">
+        <v>201</v>
+      </c>
+      <c r="F6" s="5">
+        <v>-7.9182000000000002E-3</v>
+      </c>
+      <c r="G6" s="5">
+        <v>2.0384699999999999E-2</v>
+      </c>
+      <c r="H6" s="5">
+        <v>-0.38844099999999998</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0.69810000000000005</v>
+      </c>
+      <c r="J6" s="5">
+        <v>-4.7871419999999998E-2</v>
+      </c>
+      <c r="K6" s="5">
+        <v>3.2034960000000001E-2</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="5">
+        <v>0.79504620000000004</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
@@ -3127,17 +3424,39 @@
       <c r="D7" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
+      <c r="E7" s="6">
+        <v>67</v>
+      </c>
+      <c r="F7" s="6">
+        <v>8.4329550000000003E-2</v>
+      </c>
+      <c r="G7" s="6">
+        <v>9.1927599999999998E-2</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0.91734780000000005</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0.3624</v>
+      </c>
+      <c r="J7" s="6">
+        <v>-9.5845169999999993E-2</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0.26450430000000003</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="6">
+        <v>0.48540030000000001</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
@@ -3152,17 +3471,39 @@
       <c r="D8" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
+      <c r="E8" s="9">
+        <v>61</v>
+      </c>
+      <c r="F8" s="9">
+        <v>4.7405000000000003E-2</v>
+      </c>
+      <c r="G8" s="9">
+        <v>4.3688999999999999E-2</v>
+      </c>
+      <c r="H8" s="9">
+        <v>1.0851</v>
+      </c>
+      <c r="I8" s="9">
+        <v>0.28239999999999998</v>
+      </c>
+      <c r="J8" s="9">
+        <v>-3.8223630000000001E-2</v>
+      </c>
+      <c r="K8" s="9">
+        <v>0.1330327</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="M8" s="9">
+        <v>3.5270000000000003E-2</v>
+      </c>
+      <c r="N8" s="9">
+        <v>0.21192050000000001</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="13"/>
@@ -3180,17 +3521,39 @@
       <c r="D10" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
+      <c r="E10" s="5">
+        <v>766</v>
+      </c>
+      <c r="F10" s="5">
+        <v>3.2689999999999998E-4</v>
+      </c>
+      <c r="G10" s="5">
+        <v>2.5091860000000001E-2</v>
+      </c>
+      <c r="H10" s="5">
+        <v>1.3029000000000001E-2</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0.98960000000000004</v>
+      </c>
+      <c r="J10" s="5">
+        <v>-4.885221E-2</v>
+      </c>
+      <c r="K10" s="5">
+        <v>4.9506070999999999E-2</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" s="5">
+        <v>0.38529459999999999</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
@@ -3205,17 +3568,39 @@
       <c r="D11" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
+      <c r="E11" s="6">
+        <v>127</v>
+      </c>
+      <c r="F11" s="6">
+        <v>-8.0268199999999998E-2</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.14992249999999999</v>
+      </c>
+      <c r="H11" s="6">
+        <v>-0.53539820000000005</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0.59330000000000005</v>
+      </c>
+      <c r="J11" s="6">
+        <v>-0.37411097999999998</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0.2135745</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N11" s="6">
+        <v>0.31911040000000002</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
@@ -3230,17 +3615,39 @@
       <c r="D12" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
+      <c r="E12" s="9">
+        <v>129</v>
+      </c>
+      <c r="F12" s="9">
+        <v>3.1053000000000001E-2</v>
+      </c>
+      <c r="G12" s="9">
+        <v>4.5060999999999997E-2</v>
+      </c>
+      <c r="H12" s="9">
+        <v>0.68910000000000005</v>
+      </c>
+      <c r="I12" s="9">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="J12" s="9">
+        <v>-5.7265589999999998E-2</v>
+      </c>
+      <c r="K12" s="9">
+        <v>0.11937161</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="M12" s="9">
+        <v>-1.0330000000000001E-2</v>
+      </c>
+      <c r="N12" s="39">
+        <v>2.578865E-7</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
@@ -3255,17 +3662,39 @@
       <c r="D14" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
+      <c r="E14" s="5">
+        <v>766</v>
+      </c>
+      <c r="F14" s="5">
+        <v>2.5092199999999999E-2</v>
+      </c>
+      <c r="G14" s="5">
+        <v>3.9052940000000001E-2</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0.64251800000000003</v>
+      </c>
+      <c r="I14" s="5">
+        <v>0.52070000000000005</v>
+      </c>
+      <c r="J14" s="5">
+        <v>-5.145015E-2</v>
+      </c>
+      <c r="K14" s="5">
+        <v>0.101634554</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14" s="5">
+        <v>0.38832739999999999</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
@@ -3280,17 +3709,39 @@
       <c r="D15" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
+      <c r="E15" s="6">
+        <v>127</v>
+      </c>
+      <c r="F15" s="6">
+        <v>-1.7120699999999999E-2</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0.17630109999999999</v>
+      </c>
+      <c r="H15" s="6">
+        <v>-9.7110299999999997E-2</v>
+      </c>
+      <c r="I15" s="6">
+        <v>0.92279999999999995</v>
+      </c>
+      <c r="J15" s="6">
+        <v>-0.36266453999999998</v>
+      </c>
+      <c r="K15" s="6">
+        <v>0.32842320000000003</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N15" s="6">
+        <v>0.34039550000000002</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
@@ -3305,17 +3756,39 @@
       <c r="D16" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
+      <c r="E16" s="9">
+        <v>129</v>
+      </c>
+      <c r="F16" s="9">
+        <v>7.3262999999999995E-2</v>
+      </c>
+      <c r="G16" s="9">
+        <v>8.2063999999999998E-2</v>
+      </c>
+      <c r="H16" s="9">
+        <v>0.89280000000000004</v>
+      </c>
+      <c r="I16" s="9">
+        <v>0.37369000000000002</v>
+      </c>
+      <c r="J16" s="9">
+        <v>-8.757935E-2</v>
+      </c>
+      <c r="K16" s="9">
+        <v>0.23410527</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="M16" s="9">
+        <v>-7.7679999999999997E-3</v>
+      </c>
+      <c r="N16" s="39">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>89</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3326,11 +3799,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D19BA0CD-B3A4-4C64-A7BB-E12896AEF890}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="19.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
@@ -3392,17 +3869,39 @@
       <c r="D2" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
+      <c r="E2" s="5">
+        <v>766</v>
+      </c>
+      <c r="F2" s="5">
+        <v>-9.0793299999999993E-2</v>
+      </c>
+      <c r="G2" s="5">
+        <v>4.6788860000000002E-2</v>
+      </c>
+      <c r="H2" s="5">
+        <v>-1.9404889999999999</v>
+      </c>
+      <c r="I2" s="10">
+        <v>5.2699999999999997E-2</v>
+      </c>
+      <c r="J2" s="5">
+        <v>-0.18249770000000001</v>
+      </c>
+      <c r="K2" s="5">
+        <v>9.1120610000000005E-4</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="5">
+        <v>0.37407960000000001</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
@@ -3417,17 +3916,39 @@
       <c r="D3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
+      <c r="E3" s="6">
+        <v>127</v>
+      </c>
+      <c r="F3" s="6">
+        <v>-0.15269679999999999</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0.2651501</v>
+      </c>
+      <c r="H3" s="6">
+        <v>-0.57588799999999996</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0.56569999999999998</v>
+      </c>
+      <c r="J3" s="6">
+        <v>-0.67238147999999998</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0.36698789999999998</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="6">
+        <v>0.32825749999999998</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
@@ -3442,17 +3963,39 @@
       <c r="D4" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
+      <c r="E4" s="9">
+        <v>129</v>
+      </c>
+      <c r="F4" s="9">
+        <v>7.6146000000000005E-2</v>
+      </c>
+      <c r="G4" s="9">
+        <v>7.2042999999999996E-2</v>
+      </c>
+      <c r="H4" s="9">
+        <v>1.0569999999999999</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0.29260000000000003</v>
+      </c>
+      <c r="J4" s="9">
+        <v>-6.5055959999999996E-2</v>
+      </c>
+      <c r="K4" s="9">
+        <v>0.21734832000000001</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="M4" s="9">
+        <v>-5.2300000000000003E-3</v>
+      </c>
+      <c r="N4" s="39">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="13"/>
@@ -3470,17 +4013,39 @@
       <c r="D6" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
+      <c r="E6" s="5">
+        <v>766</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.1087743</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0.1109221</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0.98063699999999998</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0.3271</v>
+      </c>
+      <c r="J6" s="5">
+        <v>-0.10862906</v>
+      </c>
+      <c r="K6" s="5">
+        <v>0.32617759950000003</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="5">
+        <v>0.38720739999999998</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
@@ -3495,17 +4060,39 @@
       <c r="D7" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
+      <c r="E7" s="6">
+        <v>127</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1.6066643</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0.60715799999999998</v>
+      </c>
+      <c r="H7" s="6">
+        <v>2.6462050000000001</v>
+      </c>
+      <c r="I7" s="11">
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0.41665651999999997</v>
+      </c>
+      <c r="K7" s="6">
+        <v>2.7966720999999999</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="6">
+        <v>0.2152647</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
@@ -3520,17 +4107,39 @@
       <c r="D8" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
+      <c r="E8" s="9">
+        <v>129</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0.45727410000000002</v>
+      </c>
+      <c r="G8" s="9">
+        <v>0.1675944</v>
+      </c>
+      <c r="H8" s="9">
+        <v>2.7284999999999999</v>
+      </c>
+      <c r="I8" s="12">
+        <v>7.273E-3</v>
+      </c>
+      <c r="J8" s="9">
+        <v>0.128795198</v>
+      </c>
+      <c r="K8" s="9">
+        <v>0.78575309000000004</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="M8" s="9">
+        <v>4.2430000000000002E-2</v>
+      </c>
+      <c r="N8" s="39">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="13"/>
@@ -3547,13 +4156,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0232423-D4EE-4B15-B8EC-2DF31E8640A1}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="19.90625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3613,17 +4225,39 @@
       <c r="D2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
+      <c r="E2" s="5">
+        <v>798</v>
+      </c>
+      <c r="F2" s="5">
+        <v>-3.5299200000000003E-2</v>
+      </c>
+      <c r="G2" s="5">
+        <v>2.2444100000000002E-2</v>
+      </c>
+      <c r="H2" s="5">
+        <v>-1.5727610000000001</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0.1162</v>
+      </c>
+      <c r="J2" s="5">
+        <v>-7.9288839999999999E-2</v>
+      </c>
+      <c r="K2" s="5">
+        <v>8.6904349999999998E-3</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="5">
+        <v>0.35023149999999997</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
@@ -3638,17 +4272,39 @@
       <c r="D3" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
+      <c r="E3" s="6">
+        <v>130</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.13424430000000001</v>
+      </c>
+      <c r="G3" s="6">
+        <v>9.79709E-2</v>
+      </c>
+      <c r="H3" s="6">
+        <v>1.3702460000000001</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="J3" s="6">
+        <v>-5.7775199999999999E-2</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0.32626369999999999</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="6">
+        <v>0.29118569999999999</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
@@ -3663,17 +4319,39 @@
       <c r="D4" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
+      <c r="E4" s="9">
+        <v>129</v>
+      </c>
+      <c r="F4" s="9">
+        <v>1.1051E-2</v>
+      </c>
+      <c r="G4" s="9">
+        <v>2.3737999999999999E-2</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0.46550000000000002</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0.64236000000000004</v>
+      </c>
+      <c r="J4" s="9">
+        <v>-3.5475698999999999E-2</v>
+      </c>
+      <c r="K4" s="9">
+        <v>5.757702E-2</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="M4" s="9">
+        <v>-6.1570000000000001E-3</v>
+      </c>
+      <c r="N4" s="39">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="13"/>

</xml_diff>

<commit_message>
final commit for the night zzz
</commit_message>
<xml_diff>
--- a/Results/Update Coastal_RESULTS.xlsx
+++ b/Results/Update Coastal_RESULTS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/emgarris_calpoly_edu/Documents/R_Projects/CoastalBirdsUPDATE/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1377" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9AD8122-E678-4A47-A10A-C285BADC815F}"/>
+  <xr:revisionPtr revIDLastSave="1380" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E074AB6-F908-4918-A67B-3F754022A258}"/>
   <bookViews>
-    <workbookView xWindow="4550" yWindow="1890" windowWidth="14440" windowHeight="8200" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sensory" sheetId="4" r:id="rId1"/>
@@ -458,7 +458,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -529,11 +529,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -602,7 +635,6 @@
     <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -614,6 +646,23 @@
     <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -900,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F82655-FE3A-4F4B-B446-2D913CF0CC8B}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1265,9 +1314,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C8F29B3-A633-40B8-A222-FC489EFBC75D}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O13" sqref="O13"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1284,7 +1333,7 @@
     <col min="14" max="14" width="9.08984375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" s="13" customFormat="1" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1912,9 +1961,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8E188F-C842-439D-93EC-074F9278CAC0}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K20" sqref="K20"/>
+      <selection pane="bottomLeft" activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1923,7 +1972,9 @@
     <col min="4" max="4" width="18.54296875" customWidth="1"/>
     <col min="6" max="6" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="8.7265625" style="4"/>
+    <col min="8" max="8" width="8.7265625" style="4"/>
+    <col min="9" max="9" width="8.7265625" style="55"/>
+    <col min="10" max="10" width="8.7265625" style="4"/>
     <col min="11" max="11" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
@@ -1952,13 +2003,13 @@
       <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="50" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="15" t="s">
@@ -2002,7 +2053,7 @@
       <c r="H2" s="17">
         <v>-2.0745309999999999</v>
       </c>
-      <c r="I2" s="37">
+      <c r="I2" s="52">
         <v>3.8600000000000002E-2</v>
       </c>
       <c r="J2" s="17">
@@ -2049,7 +2100,7 @@
       <c r="H3" s="8">
         <v>-1.0621267999999999</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="53">
         <v>0.2903</v>
       </c>
       <c r="J3" s="8">
@@ -2096,7 +2147,7 @@
       <c r="H4" s="19">
         <v>-0.36749999999999999</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="54">
         <v>0.71399999999999997</v>
       </c>
       <c r="J4" s="19">
@@ -2146,7 +2197,7 @@
       <c r="H6" s="17">
         <v>3.4458980000000001</v>
       </c>
-      <c r="I6" s="37">
+      <c r="I6" s="52">
         <v>5.9999999999999995E-4</v>
       </c>
       <c r="J6" s="17">
@@ -2193,7 +2244,7 @@
       <c r="H7" s="8">
         <v>0.90135600000000005</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="53">
         <v>0.36919999999999997</v>
       </c>
       <c r="J7" s="8">
@@ -2240,7 +2291,7 @@
       <c r="H8" s="19">
         <v>-1.0096000000000001</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="54">
         <v>0.31474999999999997</v>
       </c>
       <c r="J8" s="19">
@@ -2290,7 +2341,7 @@
       <c r="H10" s="17">
         <v>-1.3172999999999999</v>
       </c>
-      <c r="I10" s="38">
+      <c r="I10" s="56">
         <v>0.18809999999999999</v>
       </c>
       <c r="J10" s="17">
@@ -2337,7 +2388,7 @@
       <c r="H11" s="8">
         <v>-0.85048360000000001</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="53">
         <v>0.3967</v>
       </c>
       <c r="J11" s="8">
@@ -2384,7 +2435,7 @@
       <c r="H12" s="19">
         <v>-0.21740000000000001</v>
       </c>
-      <c r="I12" s="19">
+      <c r="I12" s="54">
         <v>0.82823000000000002</v>
       </c>
       <c r="J12" s="19">
@@ -2431,7 +2482,7 @@
       <c r="H14" s="17">
         <v>-0.24134900000000001</v>
       </c>
-      <c r="I14" s="17">
+      <c r="I14" s="57">
         <v>0.80930000000000002</v>
       </c>
       <c r="J14" s="17">
@@ -2478,7 +2529,7 @@
       <c r="H15" s="8">
         <v>2.1584449999999999</v>
       </c>
-      <c r="I15" s="34">
+      <c r="I15" s="58">
         <v>3.2800000000000003E-2</v>
       </c>
       <c r="J15" s="8">
@@ -2525,7 +2576,7 @@
       <c r="H16" s="19">
         <v>1.5656000000000001</v>
       </c>
-      <c r="I16" s="35">
+      <c r="I16" s="59">
         <v>0.11990000000000001</v>
       </c>
       <c r="J16" s="19">
@@ -2736,7 +2787,7 @@
       <c r="H4" s="19">
         <v>-1.4129</v>
       </c>
-      <c r="I4" s="40">
+      <c r="I4" s="39">
         <v>0.16028999999999999</v>
       </c>
       <c r="J4" s="19">
@@ -2751,7 +2802,7 @@
       <c r="M4" s="9">
         <v>1.4090000000000001E-3</v>
       </c>
-      <c r="N4" s="39">
+      <c r="N4" s="38">
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="O4" s="9" t="s">
@@ -2786,7 +2837,7 @@
       <c r="H6" s="17">
         <v>3.4888439999999998</v>
       </c>
-      <c r="I6" s="41">
+      <c r="I6" s="40">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="J6" s="17">
@@ -2880,7 +2931,7 @@
       <c r="H8" s="19">
         <v>2.1779000000000002</v>
       </c>
-      <c r="I8" s="40">
+      <c r="I8" s="39">
         <v>3.1280000000000002E-2</v>
       </c>
       <c r="J8" s="19">
@@ -2895,7 +2946,7 @@
       <c r="M8" s="9">
         <v>2.265E-2</v>
       </c>
-      <c r="N8" s="39">
+      <c r="N8" s="38">
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="O8" s="9" t="s">
@@ -3003,46 +3054,46 @@
       <c r="A12" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="44">
+      <c r="E12" s="43">
         <v>122</v>
       </c>
-      <c r="F12" s="47">
+      <c r="F12" s="46">
         <v>-0.247531</v>
       </c>
-      <c r="G12" s="47">
+      <c r="G12" s="46">
         <v>0.17519100000000001</v>
       </c>
-      <c r="H12" s="47">
+      <c r="H12" s="46">
         <v>-1.4129</v>
       </c>
-      <c r="I12" s="48">
+      <c r="I12" s="47">
         <v>0.16028999999999999</v>
       </c>
-      <c r="J12" s="47">
+      <c r="J12" s="46">
         <v>-0.59089959999999997</v>
       </c>
-      <c r="K12" s="47">
+      <c r="K12" s="46">
         <v>9.5837240000000004E-2</v>
       </c>
-      <c r="L12" s="44">
+      <c r="L12" s="43">
         <v>1.7909999999999999E-2</v>
       </c>
-      <c r="M12" s="44">
+      <c r="M12" s="43">
         <v>1.4090000000000001E-3</v>
       </c>
-      <c r="N12" s="46">
+      <c r="N12" s="45">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="O12" s="44" t="s">
+      <c r="O12" s="43" t="s">
         <v>68</v>
       </c>
     </row>
@@ -3165,7 +3216,7 @@
       <c r="H16" s="19">
         <v>2.0190999999999999</v>
       </c>
-      <c r="I16" s="40">
+      <c r="I16" s="39">
         <v>4.5600000000000002E-2</v>
       </c>
       <c r="J16" s="19">
@@ -3180,7 +3231,7 @@
       <c r="M16" s="9">
         <v>1.7639999999999999E-2</v>
       </c>
-      <c r="N16" s="39">
+      <c r="N16" s="38">
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="O16" s="9" t="s">
@@ -3676,7 +3727,7 @@
       <c r="M12" s="9">
         <v>-1.0330000000000001E-2</v>
       </c>
-      <c r="N12" s="39">
+      <c r="N12" s="38">
         <v>2.578865E-7</v>
       </c>
       <c r="O12" s="9" t="s">
@@ -3817,7 +3868,7 @@
       <c r="M16" s="9">
         <v>-7.7679999999999997E-3</v>
       </c>
-      <c r="N16" s="39">
+      <c r="N16" s="38">
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="O16" s="9" t="s">
@@ -3833,9 +3884,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D19BA0CD-B3A4-4C64-A7BB-E12896AEF890}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N10" sqref="N10"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3962,7 +4013,7 @@
       <c r="H3" s="6">
         <v>-1.3003813</v>
       </c>
-      <c r="I3" s="49">
+      <c r="I3" s="48">
         <v>0.19600000000000001</v>
       </c>
       <c r="J3" s="6">
@@ -4024,7 +4075,7 @@
       <c r="M4" s="9">
         <v>-9.7959999999999992E-3</v>
       </c>
-      <c r="N4" s="39">
+      <c r="N4" s="38">
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="O4" s="9" t="s">
@@ -4085,46 +4136,46 @@
       <c r="A7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="42">
+      <c r="E7" s="41">
         <v>127</v>
       </c>
-      <c r="F7" s="42">
+      <c r="F7" s="41">
         <v>1.6066643</v>
       </c>
-      <c r="G7" s="42">
+      <c r="G7" s="41">
         <v>0.60715799999999998</v>
       </c>
-      <c r="H7" s="42">
+      <c r="H7" s="41">
         <v>2.6462050000000001</v>
       </c>
-      <c r="I7" s="43">
+      <c r="I7" s="42">
         <v>9.1999999999999998E-3</v>
       </c>
-      <c r="J7" s="42">
+      <c r="J7" s="41">
         <v>0.41665651999999997</v>
       </c>
-      <c r="K7" s="42">
+      <c r="K7" s="41">
         <v>2.7966720999999999</v>
       </c>
-      <c r="L7" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="N7" s="42">
+      <c r="L7" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="41">
         <v>0.2152647</v>
       </c>
-      <c r="O7" s="42" t="s">
+      <c r="O7" s="41" t="s">
         <v>93</v>
       </c>
     </row>
@@ -4132,46 +4183,46 @@
       <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="E8" s="44">
+      <c r="E8" s="43">
         <v>129</v>
       </c>
-      <c r="F8" s="44">
+      <c r="F8" s="43">
         <v>0.45727410000000002</v>
       </c>
-      <c r="G8" s="44">
+      <c r="G8" s="43">
         <v>0.1675944</v>
       </c>
-      <c r="H8" s="44">
+      <c r="H8" s="43">
         <v>2.7284999999999999</v>
       </c>
-      <c r="I8" s="45">
+      <c r="I8" s="44">
         <v>7.273E-3</v>
       </c>
-      <c r="J8" s="44">
+      <c r="J8" s="43">
         <v>0.128795198</v>
       </c>
-      <c r="K8" s="44">
+      <c r="K8" s="43">
         <v>0.78575309000000004</v>
       </c>
-      <c r="L8" s="44" t="s">
+      <c r="L8" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="M8" s="44">
+      <c r="M8" s="43">
         <v>4.2430000000000002E-2</v>
       </c>
-      <c r="N8" s="46">
+      <c r="N8" s="45">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="O8" s="44" t="s">
+      <c r="O8" s="43" t="s">
         <v>94</v>
       </c>
     </row>
@@ -4381,7 +4432,7 @@
       <c r="M4" s="9">
         <v>-6.1570000000000001E-3</v>
       </c>
-      <c r="N4" s="39">
+      <c r="N4" s="38">
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="O4" s="9" t="s">

</xml_diff>

<commit_message>
Created FIGURES_results.R script, and also corrected boxplots for binomial predictor trait models.
</commit_message>
<xml_diff>
--- a/Results/Update Coastal_RESULTS.xlsx
+++ b/Results/Update Coastal_RESULTS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/emgarris_calpoly_edu/Documents/R_Projects/CoastalBirdsUPDATE/Results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1c136e7e6be00f1/Desktop/CoastalBirdsUPDATE/CoastalBirdsUPDATE/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1527" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7616CCA-B01B-4347-B43A-B31D0AEF2578}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sensory" sheetId="4" r:id="rId1"/>
@@ -630,7 +630,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -727,11 +727,8 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -745,8 +742,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -765,10 +760,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2048,9 +2039,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8E188F-C842-439D-93EC-074F9278CAC0}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2694,7 +2685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA225CA-067B-4F77-85FD-EE40FC6CFFCC}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N17" sqref="N17"/>
     </sheetView>
@@ -2875,7 +2866,7 @@
       <c r="H4" s="19">
         <v>-0.65800000000000003</v>
       </c>
-      <c r="I4" s="78">
+      <c r="I4" s="19">
         <v>0.51180000000000003</v>
       </c>
       <c r="J4" s="19">
@@ -2897,154 +2888,149 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="61" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="60"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
-      <c r="N5" s="64"/>
-    </row>
-    <row r="6" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="65" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" s="13"/>
+      <c r="I5" s="60"/>
+      <c r="N5" s="61"/>
+    </row>
+    <row r="6" spans="1:15" s="63" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="66" t="s">
+      <c r="C6" s="63" t="s">
         <v>99</v>
       </c>
-      <c r="D6" s="66" t="s">
+      <c r="D6" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="66">
+      <c r="E6" s="63">
         <v>575</v>
       </c>
-      <c r="F6" s="67">
+      <c r="F6" s="64">
         <v>-0.2226281</v>
       </c>
-      <c r="G6" s="67">
+      <c r="G6" s="64">
         <v>6.7531720000000003E-2</v>
       </c>
-      <c r="H6" s="67">
+      <c r="H6" s="64">
         <v>-3.2966449999999998</v>
       </c>
-      <c r="I6" s="68">
+      <c r="I6" s="65">
         <v>1E-3</v>
       </c>
-      <c r="J6" s="67">
+      <c r="J6" s="64">
         <v>-0.35498781000000001</v>
       </c>
-      <c r="K6" s="67">
+      <c r="K6" s="64">
         <v>-9.0268349999999997E-2</v>
       </c>
-      <c r="L6" s="66" t="s">
-        <v>27</v>
-      </c>
-      <c r="M6" s="66" t="s">
-        <v>27</v>
-      </c>
-      <c r="N6" s="67">
+      <c r="L6" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="64">
         <v>0.14573320000000001</v>
       </c>
-      <c r="O6" s="66" t="s">
+      <c r="O6" s="63" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="71" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="70" t="s">
+    <row r="7" spans="1:15" s="68" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="71" t="s">
+      <c r="C7" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="D7" s="71" t="s">
+      <c r="D7" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="71">
+      <c r="E7" s="68">
         <v>91</v>
       </c>
-      <c r="F7" s="72">
+      <c r="F7" s="69">
         <v>-0.72873929999999998</v>
       </c>
-      <c r="G7" s="72">
+      <c r="G7" s="69">
         <v>0.35372100000000001</v>
       </c>
-      <c r="H7" s="72">
+      <c r="H7" s="69">
         <v>-2.0602094000000002</v>
       </c>
-      <c r="I7" s="73">
+      <c r="I7" s="70">
         <v>4.2299999999999997E-2</v>
       </c>
-      <c r="J7" s="72">
+      <c r="J7" s="69">
         <v>-1.4220196899999999</v>
       </c>
-      <c r="K7" s="72">
+      <c r="K7" s="69">
         <v>-3.5458910000000003E-2</v>
       </c>
-      <c r="L7" s="71" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" s="71" t="s">
-        <v>27</v>
-      </c>
-      <c r="N7" s="72">
+      <c r="L7" s="68" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="68" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="69">
         <v>0.3</v>
       </c>
-      <c r="O7" s="71" t="s">
+      <c r="O7" s="68" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="75" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="74" t="s">
+    <row r="8" spans="1:15" s="72" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="75" t="s">
+      <c r="C8" s="72" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="75" t="s">
+      <c r="D8" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="75">
+      <c r="E8" s="72">
         <v>104</v>
       </c>
-      <c r="F8" s="76">
+      <c r="F8" s="73">
         <v>-0.120382</v>
       </c>
-      <c r="G8" s="76">
+      <c r="G8" s="73">
         <v>0.109667</v>
       </c>
-      <c r="H8" s="76">
+      <c r="H8" s="73">
         <v>-1.0976999999999999</v>
       </c>
-      <c r="I8" s="79">
+      <c r="I8" s="73">
         <v>0.27494000000000002</v>
       </c>
-      <c r="J8" s="76">
+      <c r="J8" s="73">
         <v>-0.33532611000000001</v>
       </c>
-      <c r="K8" s="76">
+      <c r="K8" s="73">
         <v>9.4561439999999997E-2</v>
       </c>
-      <c r="L8" s="75" t="s">
+      <c r="L8" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="M8" s="75">
+      <c r="M8" s="72">
         <v>-7.77E-3</v>
       </c>
-      <c r="N8" s="77">
+      <c r="N8" s="74">
         <v>2.036871E-3</v>
       </c>
-      <c r="O8" s="75" t="s">
+      <c r="O8" s="72" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3076,7 +3062,7 @@
       <c r="H10" s="17">
         <v>3.4888439999999998</v>
       </c>
-      <c r="I10" s="80">
+      <c r="I10" s="75">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="J10" s="17">
@@ -3192,154 +3178,149 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="61" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="60"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="63"/>
-      <c r="J13" s="62"/>
-      <c r="K13" s="62"/>
-      <c r="N13" s="64"/>
-    </row>
-    <row r="14" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="65" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" s="13"/>
+      <c r="I13" s="60"/>
+      <c r="N13" s="61"/>
+    </row>
+    <row r="14" spans="1:15" s="63" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="66" t="s">
+      <c r="B14" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="66" t="s">
+      <c r="C14" s="63" t="s">
         <v>99</v>
       </c>
-      <c r="D14" s="66" t="s">
+      <c r="D14" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="66">
+      <c r="E14" s="63">
         <v>575</v>
       </c>
-      <c r="F14" s="67">
+      <c r="F14" s="64">
         <v>0.214503</v>
       </c>
-      <c r="G14" s="67">
+      <c r="G14" s="64">
         <v>6.7277190000000001E-2</v>
       </c>
-      <c r="H14" s="67">
+      <c r="H14" s="64">
         <v>3.1883469999999998</v>
       </c>
-      <c r="I14" s="81">
+      <c r="I14" s="76">
         <v>1.5E-3</v>
       </c>
-      <c r="J14" s="67">
+      <c r="J14" s="64">
         <v>8.2642160000000006E-2</v>
       </c>
-      <c r="K14" s="67">
+      <c r="K14" s="64">
         <v>0.3463639</v>
       </c>
-      <c r="L14" s="66" t="s">
-        <v>27</v>
-      </c>
-      <c r="M14" s="66" t="s">
-        <v>27</v>
-      </c>
-      <c r="N14" s="69">
+      <c r="L14" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="M14" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14" s="66">
         <v>0.1434502</v>
       </c>
-      <c r="O14" s="66" t="s">
+      <c r="O14" s="63" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="71" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="70" t="s">
+    <row r="15" spans="1:15" s="68" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="71" t="s">
+      <c r="B15" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="71" t="s">
+      <c r="C15" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="D15" s="71" t="s">
+      <c r="D15" s="68" t="s">
         <v>104</v>
       </c>
-      <c r="E15" s="71">
+      <c r="E15" s="68">
         <v>91</v>
       </c>
-      <c r="F15" s="72">
+      <c r="F15" s="69">
         <v>0.72873929999999998</v>
       </c>
-      <c r="G15" s="72">
+      <c r="G15" s="69">
         <v>0.35372100000000001</v>
       </c>
-      <c r="H15" s="72">
+      <c r="H15" s="69">
         <v>2.060209</v>
       </c>
-      <c r="I15" s="73">
+      <c r="I15" s="70">
         <v>4.2299999999999997E-2</v>
       </c>
-      <c r="J15" s="72">
+      <c r="J15" s="69">
         <v>3.5458910000000003E-2</v>
       </c>
-      <c r="K15" s="72">
+      <c r="K15" s="69">
         <v>1.4220197000000001</v>
       </c>
-      <c r="L15" s="71" t="s">
-        <v>27</v>
-      </c>
-      <c r="M15" s="71" t="s">
-        <v>27</v>
-      </c>
-      <c r="N15" s="82">
+      <c r="L15" s="68" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="68" t="s">
+        <v>27</v>
+      </c>
+      <c r="N15" s="77">
         <v>0.3</v>
       </c>
-      <c r="O15" s="71" t="s">
+      <c r="O15" s="68" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="75" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="74" t="s">
+    <row r="16" spans="1:15" s="72" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="75" t="s">
+      <c r="B16" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="75" t="s">
+      <c r="C16" s="72" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="75" t="s">
+      <c r="D16" s="72" t="s">
         <v>104</v>
       </c>
-      <c r="E16" s="75">
+      <c r="E16" s="72">
         <v>104</v>
       </c>
-      <c r="F16" s="76">
+      <c r="F16" s="73">
         <v>0.120382</v>
       </c>
-      <c r="G16" s="76">
+      <c r="G16" s="73">
         <v>0.109667</v>
       </c>
-      <c r="H16" s="76">
+      <c r="H16" s="73">
         <v>1.0976999999999999</v>
       </c>
-      <c r="I16" s="79">
+      <c r="I16" s="73">
         <v>0.27489999999999998</v>
       </c>
-      <c r="J16" s="76">
+      <c r="J16" s="73">
         <v>-9.4561439999999997E-2</v>
       </c>
-      <c r="K16" s="76">
+      <c r="K16" s="73">
         <v>0.33532611000000001</v>
       </c>
-      <c r="L16" s="75" t="s">
+      <c r="L16" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="M16" s="75">
+      <c r="M16" s="72">
         <v>7.77E-3</v>
       </c>
-      <c r="N16" s="77">
+      <c r="N16" s="74">
         <v>2.036871E-3</v>
       </c>
-      <c r="O16" s="75" t="s">
+      <c r="O16" s="72" t="s">
         <v>115</v>
       </c>
     </row>

</xml_diff>

<commit_message>
plots for all besides territoriality models.
</commit_message>
<xml_diff>
--- a/Results/Update Coastal_RESULTS.xlsx
+++ b/Results/Update Coastal_RESULTS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1c136e7e6be00f1/Desktop/CoastalBirdsUPDATE/CoastalBirdsUPDATE/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1527" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7616CCA-B01B-4347-B43A-B31D0AEF2578}"/>
+  <xr:revisionPtr revIDLastSave="1531" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{358D47AF-5E77-4966-9F9D-3EBB2A97597F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sensory" sheetId="4" r:id="rId1"/>
@@ -522,7 +522,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -626,11 +626,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -729,22 +809,28 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2039,7 +2125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8E188F-C842-439D-93EC-074F9278CAC0}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
@@ -2685,9 +2771,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA225CA-067B-4F77-85FD-EE40FC6CFFCC}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N17" sqref="N17"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2888,149 +2974,149 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="13"/>
       <c r="I5" s="60"/>
       <c r="N5" s="61"/>
     </row>
-    <row r="6" spans="1:15" s="63" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="62" t="s">
+    <row r="6" spans="1:15" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="70" t="s">
         <v>99</v>
       </c>
-      <c r="D6" s="63" t="s">
+      <c r="D6" s="70" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="63">
+      <c r="E6" s="70">
         <v>575</v>
       </c>
-      <c r="F6" s="64">
+      <c r="F6" s="71">
         <v>-0.2226281</v>
       </c>
-      <c r="G6" s="64">
+      <c r="G6" s="71">
         <v>6.7531720000000003E-2</v>
       </c>
-      <c r="H6" s="64">
+      <c r="H6" s="71">
         <v>-3.2966449999999998</v>
       </c>
-      <c r="I6" s="65">
+      <c r="I6" s="72">
         <v>1E-3</v>
       </c>
-      <c r="J6" s="64">
+      <c r="J6" s="71">
         <v>-0.35498781000000001</v>
       </c>
-      <c r="K6" s="64">
+      <c r="K6" s="71">
         <v>-9.0268349999999997E-2</v>
       </c>
-      <c r="L6" s="63" t="s">
-        <v>27</v>
-      </c>
-      <c r="M6" s="63" t="s">
-        <v>27</v>
-      </c>
-      <c r="N6" s="64">
+      <c r="L6" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="71">
         <v>0.14573320000000001</v>
       </c>
-      <c r="O6" s="63" t="s">
+      <c r="O6" s="73" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="68" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="67" t="s">
+    <row r="7" spans="1:15" s="63" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="68" t="s">
+      <c r="C7" s="66" t="s">
         <v>99</v>
       </c>
-      <c r="D7" s="68" t="s">
+      <c r="D7" s="66" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="68">
+      <c r="E7" s="66">
         <v>91</v>
       </c>
-      <c r="F7" s="69">
+      <c r="F7" s="67">
         <v>-0.72873929999999998</v>
       </c>
-      <c r="G7" s="69">
+      <c r="G7" s="67">
         <v>0.35372100000000001</v>
       </c>
-      <c r="H7" s="69">
+      <c r="H7" s="67">
         <v>-2.0602094000000002</v>
       </c>
-      <c r="I7" s="70">
+      <c r="I7" s="68">
         <v>4.2299999999999997E-2</v>
       </c>
-      <c r="J7" s="69">
+      <c r="J7" s="67">
         <v>-1.4220196899999999</v>
       </c>
-      <c r="K7" s="69">
+      <c r="K7" s="67">
         <v>-3.5458910000000003E-2</v>
       </c>
-      <c r="L7" s="68" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" s="68" t="s">
-        <v>27</v>
-      </c>
-      <c r="N7" s="69">
+      <c r="L7" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="67">
         <v>0.3</v>
       </c>
-      <c r="O7" s="68" t="s">
+      <c r="O7" s="75" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="72" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="71" t="s">
+    <row r="8" spans="1:15" s="64" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="72" t="s">
+      <c r="B8" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="72" t="s">
+      <c r="C8" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="72" t="s">
+      <c r="D8" s="77" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="72">
+      <c r="E8" s="77">
         <v>104</v>
       </c>
-      <c r="F8" s="73">
+      <c r="F8" s="78">
         <v>-0.120382</v>
       </c>
-      <c r="G8" s="73">
+      <c r="G8" s="78">
         <v>0.109667</v>
       </c>
-      <c r="H8" s="73">
+      <c r="H8" s="78">
         <v>-1.0976999999999999</v>
       </c>
-      <c r="I8" s="73">
+      <c r="I8" s="78">
         <v>0.27494000000000002</v>
       </c>
-      <c r="J8" s="73">
+      <c r="J8" s="78">
         <v>-0.33532611000000001</v>
       </c>
-      <c r="K8" s="73">
+      <c r="K8" s="78">
         <v>9.4561439999999997E-2</v>
       </c>
-      <c r="L8" s="72" t="s">
+      <c r="L8" s="77" t="s">
         <v>110</v>
       </c>
-      <c r="M8" s="72">
+      <c r="M8" s="77">
         <v>-7.77E-3</v>
       </c>
-      <c r="N8" s="74">
+      <c r="N8" s="79">
         <v>2.036871E-3</v>
       </c>
-      <c r="O8" s="72" t="s">
+      <c r="O8" s="80" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3062,7 +3148,7 @@
       <c r="H10" s="17">
         <v>3.4888439999999998</v>
       </c>
-      <c r="I10" s="75">
+      <c r="I10" s="65">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="J10" s="17">
@@ -3178,149 +3264,149 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="13"/>
       <c r="I13" s="60"/>
       <c r="N13" s="61"/>
     </row>
-    <row r="14" spans="1:15" s="63" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="62" t="s">
+    <row r="14" spans="1:15" s="70" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="63" t="s">
+      <c r="B14" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="63" t="s">
+      <c r="C14" s="70" t="s">
         <v>99</v>
       </c>
-      <c r="D14" s="63" t="s">
+      <c r="D14" s="70" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="63">
+      <c r="E14" s="70">
         <v>575</v>
       </c>
-      <c r="F14" s="64">
+      <c r="F14" s="71">
         <v>0.214503</v>
       </c>
-      <c r="G14" s="64">
+      <c r="G14" s="71">
         <v>6.7277190000000001E-2</v>
       </c>
-      <c r="H14" s="64">
+      <c r="H14" s="71">
         <v>3.1883469999999998</v>
       </c>
-      <c r="I14" s="76">
+      <c r="I14" s="81">
         <v>1.5E-3</v>
       </c>
-      <c r="J14" s="64">
+      <c r="J14" s="71">
         <v>8.2642160000000006E-2</v>
       </c>
-      <c r="K14" s="64">
+      <c r="K14" s="71">
         <v>0.3463639</v>
       </c>
-      <c r="L14" s="63" t="s">
-        <v>27</v>
-      </c>
-      <c r="M14" s="63" t="s">
-        <v>27</v>
-      </c>
-      <c r="N14" s="66">
+      <c r="L14" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="M14" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14" s="82">
         <v>0.1434502</v>
       </c>
-      <c r="O14" s="63" t="s">
+      <c r="O14" s="70" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="68" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="67" t="s">
+    <row r="15" spans="1:15" s="66" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="68" t="s">
+      <c r="B15" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="68" t="s">
+      <c r="C15" s="66" t="s">
         <v>99</v>
       </c>
-      <c r="D15" s="68" t="s">
+      <c r="D15" s="66" t="s">
         <v>104</v>
       </c>
-      <c r="E15" s="68">
+      <c r="E15" s="66">
         <v>91</v>
       </c>
-      <c r="F15" s="69">
+      <c r="F15" s="67">
         <v>0.72873929999999998</v>
       </c>
-      <c r="G15" s="69">
+      <c r="G15" s="67">
         <v>0.35372100000000001</v>
       </c>
-      <c r="H15" s="69">
+      <c r="H15" s="67">
         <v>2.060209</v>
       </c>
-      <c r="I15" s="70">
+      <c r="I15" s="68">
         <v>4.2299999999999997E-2</v>
       </c>
-      <c r="J15" s="69">
+      <c r="J15" s="67">
         <v>3.5458910000000003E-2</v>
       </c>
-      <c r="K15" s="69">
+      <c r="K15" s="67">
         <v>1.4220197000000001</v>
       </c>
-      <c r="L15" s="68" t="s">
-        <v>27</v>
-      </c>
-      <c r="M15" s="68" t="s">
-        <v>27</v>
-      </c>
-      <c r="N15" s="77">
+      <c r="L15" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="N15" s="83">
         <v>0.3</v>
       </c>
-      <c r="O15" s="68" t="s">
+      <c r="O15" s="66" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="72" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="71" t="s">
+    <row r="16" spans="1:15" s="77" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="72" t="s">
+      <c r="B16" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="72" t="s">
+      <c r="C16" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="72" t="s">
+      <c r="D16" s="77" t="s">
         <v>104</v>
       </c>
-      <c r="E16" s="72">
+      <c r="E16" s="77">
         <v>104</v>
       </c>
-      <c r="F16" s="73">
+      <c r="F16" s="78">
         <v>0.120382</v>
       </c>
-      <c r="G16" s="73">
+      <c r="G16" s="78">
         <v>0.109667</v>
       </c>
-      <c r="H16" s="73">
+      <c r="H16" s="78">
         <v>1.0976999999999999</v>
       </c>
-      <c r="I16" s="73">
+      <c r="I16" s="78">
         <v>0.27489999999999998</v>
       </c>
-      <c r="J16" s="73">
+      <c r="J16" s="78">
         <v>-9.4561439999999997E-2</v>
       </c>
-      <c r="K16" s="73">
+      <c r="K16" s="78">
         <v>0.33532611000000001</v>
       </c>
-      <c r="L16" s="72" t="s">
+      <c r="L16" s="77" t="s">
         <v>110</v>
       </c>
-      <c r="M16" s="72">
+      <c r="M16" s="77">
         <v>7.77E-3</v>
       </c>
-      <c r="N16" s="74">
+      <c r="N16" s="79">
         <v>2.036871E-3</v>
       </c>
-      <c r="O16" s="72" t="s">
+      <c r="O16" s="77" t="s">
         <v>115</v>
       </c>
     </row>

</xml_diff>

<commit_message>
redid some results figures and created new ones. 1/2 done - resume on 10.2.24
</commit_message>
<xml_diff>
--- a/Results/Update Coastal_RESULTS.xlsx
+++ b/Results/Update Coastal_RESULTS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1c136e7e6be00f1/Desktop/CoastalBirdsUPDATE/CoastalBirdsUPDATE/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2562" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E3CD8C4-46E3-4658-B4A2-D6BE250457F4}"/>
+  <xr:revisionPtr revIDLastSave="2684" documentId="11_F25DC773A252ABDACC104805699D74C65BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C082D97-246C-4CE3-ADC5-86853BBFEEFE}"/>
   <bookViews>
-    <workbookView xWindow="10480" yWindow="0" windowWidth="8740" windowHeight="11270" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12250" yWindow="0" windowWidth="7040" windowHeight="11010" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sensory" sheetId="4" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="140">
   <si>
     <t>Index used</t>
   </si>
@@ -395,9 +395,6 @@
     <t>histograms of binomial distributions and q-q look fine</t>
   </si>
   <si>
-    <t xml:space="preserve"> q-q plot doing weird thing associated with "alpha reached uppoer bound" warning. </t>
-  </si>
-  <si>
     <t>------</t>
   </si>
   <si>
@@ -435,6 +432,36 @@
   </si>
   <si>
     <t xml:space="preserve">RE-EVALUATE C.I. (depending on Sarah's Email) --&gt; yellow highlight instead of blue highlight? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">phyglm_UN_nest_low_fix --&gt;  scaled variables, alpha forced near/at upper bounds </t>
+  </si>
+  <si>
+    <t xml:space="preserve">phyglm_UN_nest_low_only_scale --&gt; scaled variables </t>
+  </si>
+  <si>
+    <t xml:space="preserve">even though p value flagged as significant, bootstrapped CI crosses over 0… the other CI (yellow) does not cross 0… </t>
+  </si>
+  <si>
+    <t>phyglm_UN_nest_high_fix --&gt; scaled variables, alpha forced near/at upper bounds</t>
+  </si>
+  <si>
+    <t>phyglm_UN_nest_high_only_scale --&gt; scaled variables</t>
+  </si>
+  <si>
+    <t>phyglm_UN_brightness_scale --&gt; scaled variables</t>
+  </si>
+  <si>
+    <t>phyglm_UN_hue_scale --&gt; scaled variables</t>
+  </si>
+  <si>
+    <t>phyglm_UN_ssm_fix --&gt; scaled variables, alpha forced near/at upper bounds</t>
+  </si>
+  <si>
+    <t>phyglm_UN_ssf_fix_4.05 --&gt; scaled variables, alpha forced near/at upper bounds, had to go slightly above 4 for log.alpha.bound to get a model that would converge</t>
+  </si>
+  <si>
+    <t>phyglm_UN_territorial_scale --&gt; scaled variables</t>
   </si>
 </sst>
 </file>
@@ -529,7 +556,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -587,6 +614,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF85DFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -790,7 +823,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -909,7 +942,6 @@
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="4" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -995,7 +1027,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="5" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1014,10 +1045,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1378,7 +1420,7 @@
       <c r="P1" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="110" t="s">
+      <c r="Q1" s="109" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1416,19 +1458,19 @@
       <c r="K2" s="16">
         <v>1.458</v>
       </c>
-      <c r="L2" s="109" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="109" t="s">
+      <c r="L2" s="108" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="108" t="s">
         <v>27</v>
       </c>
       <c r="N2" s="17">
         <v>0</v>
       </c>
-      <c r="O2" s="109" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="109" t="s">
+      <c r="O2" s="108" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="108" t="s">
         <v>27</v>
       </c>
       <c r="Q2" s="5" t="s">
@@ -1469,19 +1511,19 @@
       <c r="K3" s="8">
         <v>7.0210509999999999</v>
       </c>
-      <c r="L3" s="93" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="93" t="s">
+      <c r="L3" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="92" t="s">
         <v>27</v>
       </c>
       <c r="N3" s="8">
         <v>0.1</v>
       </c>
-      <c r="O3" s="93" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" s="93" t="s">
+      <c r="O3" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" s="92" t="s">
         <v>27</v>
       </c>
       <c r="Q3" s="6" t="s">
@@ -1528,13 +1570,13 @@
       <c r="M4" s="19">
         <v>-1.8190000000000001E-2</v>
       </c>
-      <c r="N4" s="94" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" s="94">
+      <c r="N4" s="93" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" s="93">
         <v>0</v>
       </c>
-      <c r="P4" s="94" t="s">
+      <c r="P4" s="93" t="s">
         <v>27</v>
       </c>
       <c r="Q4" s="9" t="s">
@@ -1551,13 +1593,13 @@
       <c r="C5" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="88" t="s">
+      <c r="D5" s="87" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="79">
         <v>38</v>
       </c>
-      <c r="F5" s="89">
+      <c r="F5" s="88">
         <v>-0.11899999999999999</v>
       </c>
       <c r="G5" s="82">
@@ -1581,7 +1623,7 @@
       <c r="M5" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="N5" s="95" t="s">
+      <c r="N5" s="94" t="s">
         <v>27</v>
       </c>
       <c r="O5" s="82">
@@ -1591,7 +1633,7 @@
         <v>1.798</v>
       </c>
       <c r="Q5" s="79" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
@@ -1620,7 +1662,7 @@
       <c r="G7" s="21">
         <v>4.07E-5</v>
       </c>
-      <c r="H7" s="108">
+      <c r="H7" s="107">
         <v>-1.0410079999999999</v>
       </c>
       <c r="I7" s="16">
@@ -1632,19 +1674,19 @@
       <c r="K7" s="22">
         <v>3.7381359999999998E-5</v>
       </c>
-      <c r="L7" s="109" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" s="109" t="s">
+      <c r="L7" s="108" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="108" t="s">
         <v>27</v>
       </c>
       <c r="N7" s="17">
         <v>0.72</v>
       </c>
-      <c r="O7" s="109" t="s">
-        <v>27</v>
-      </c>
-      <c r="P7" s="109" t="s">
+      <c r="O7" s="108" t="s">
+        <v>27</v>
+      </c>
+      <c r="P7" s="108" t="s">
         <v>27</v>
       </c>
       <c r="Q7" s="5" t="s">
@@ -1685,19 +1727,19 @@
       <c r="K8" s="24">
         <v>2.7208810000000001E-4</v>
       </c>
-      <c r="L8" s="93" t="s">
-        <v>27</v>
-      </c>
-      <c r="M8" s="93" t="s">
+      <c r="L8" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="92" t="s">
         <v>27</v>
       </c>
       <c r="N8" s="8">
         <v>0.1</v>
       </c>
-      <c r="O8" s="93" t="s">
-        <v>27</v>
-      </c>
-      <c r="P8" s="93" t="s">
+      <c r="O8" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="P8" s="92" t="s">
         <v>27</v>
       </c>
       <c r="Q8" s="6" t="s">
@@ -1744,13 +1786,13 @@
       <c r="M9" s="19">
         <v>-4.5820000000000001E-3</v>
       </c>
-      <c r="N9" s="94" t="s">
-        <v>27</v>
-      </c>
-      <c r="O9" s="98">
+      <c r="N9" s="93" t="s">
+        <v>27</v>
+      </c>
+      <c r="O9" s="97">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="P9" s="94" t="s">
+      <c r="P9" s="93" t="s">
         <v>27</v>
       </c>
       <c r="Q9" s="9" t="s">
@@ -1767,19 +1809,19 @@
       <c r="C10" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="88" t="s">
+      <c r="D10" s="87" t="s">
         <v>16</v>
       </c>
       <c r="E10" s="79">
         <v>129</v>
       </c>
-      <c r="F10" s="99">
+      <c r="F10" s="98">
         <v>2.2599999999999999E-2</v>
       </c>
-      <c r="G10" s="99">
+      <c r="G10" s="98">
         <v>0.27400000000000002</v>
       </c>
-      <c r="H10" s="99">
+      <c r="H10" s="98">
         <v>8.3400000000000002E-2</v>
       </c>
       <c r="I10" s="82">
@@ -1797,7 +1839,7 @@
       <c r="M10" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="N10" s="95" t="s">
+      <c r="N10" s="94" t="s">
         <v>27</v>
       </c>
       <c r="O10" s="82">
@@ -1806,8 +1848,8 @@
       <c r="P10" s="82">
         <v>1.2390000000000001</v>
       </c>
-      <c r="Q10" s="128" t="s">
-        <v>121</v>
+      <c r="Q10" s="126" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
@@ -1825,9 +1867,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C8F29B3-A633-40B8-A222-FC489EFBC75D}">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K22" sqref="K22"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1871,7 +1913,7 @@
       <c r="H1" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="129" t="s">
+      <c r="I1" s="127" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="44" t="s">
@@ -1933,19 +1975,19 @@
       <c r="K2" s="22">
         <v>1.3481610000000001E-3</v>
       </c>
-      <c r="L2" s="92" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="92" t="s">
+      <c r="L2" s="91" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="91" t="s">
         <v>27</v>
       </c>
       <c r="N2" s="17">
         <v>0.35207739999999998</v>
       </c>
-      <c r="O2" s="92" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="92" t="s">
+      <c r="O2" s="91" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="91" t="s">
         <v>27</v>
       </c>
       <c r="Q2" s="5" t="s">
@@ -1977,7 +2019,7 @@
       <c r="H3" s="8">
         <v>-1.9227075</v>
       </c>
-      <c r="I3" s="130">
+      <c r="I3" s="128">
         <v>5.6800000000000003E-2</v>
       </c>
       <c r="J3" s="8">
@@ -1986,19 +2028,19 @@
       <c r="K3" s="23">
         <v>1.8233029999999999E-4</v>
       </c>
-      <c r="L3" s="93" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="93" t="s">
+      <c r="L3" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="92" t="s">
         <v>27</v>
       </c>
       <c r="N3" s="8">
         <v>0.27234940000000002</v>
       </c>
-      <c r="O3" s="93" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" s="93" t="s">
+      <c r="O3" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" s="92" t="s">
         <v>27</v>
       </c>
       <c r="Q3" s="6" t="s">
@@ -2045,13 +2087,13 @@
       <c r="M4" s="19">
         <v>-1.414E-2</v>
       </c>
-      <c r="N4" s="98" t="s">
+      <c r="N4" s="97" t="s">
         <v>27</v>
       </c>
       <c r="O4" s="26">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="P4" s="98" t="s">
+      <c r="P4" s="97" t="s">
         <v>27</v>
       </c>
       <c r="Q4" s="9" t="s">
@@ -2068,13 +2110,13 @@
       <c r="C5" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="88" t="s">
+      <c r="D5" s="87" t="s">
         <v>31</v>
       </c>
       <c r="E5" s="79">
         <v>129</v>
       </c>
-      <c r="F5" s="99">
+      <c r="F5" s="98">
         <v>6.0499999999999998E-2</v>
       </c>
       <c r="G5" s="82">
@@ -2083,37 +2125,37 @@
       <c r="H5" s="82">
         <v>0.22500000000000001</v>
       </c>
-      <c r="I5" s="91">
+      <c r="I5" s="90">
         <v>0.82199999999999995</v>
       </c>
       <c r="J5" s="82">
         <v>-0.378</v>
       </c>
-      <c r="K5" s="99">
+      <c r="K5" s="98">
         <v>0.47599999999999998</v>
       </c>
-      <c r="L5" s="100" t="s">
-        <v>27</v>
-      </c>
-      <c r="M5" s="100" t="s">
-        <v>27</v>
-      </c>
-      <c r="N5" s="100" t="s">
-        <v>27</v>
-      </c>
-      <c r="O5" s="99">
+      <c r="L5" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5" s="98">
         <v>0.58599999999999997</v>
       </c>
       <c r="P5" s="82">
         <v>1.1830000000000001</v>
       </c>
       <c r="Q5" s="79" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="13"/>
-      <c r="N6" s="101"/>
+      <c r="N6" s="100"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
@@ -2149,19 +2191,19 @@
       <c r="K7" s="22">
         <v>2.2639320000000002E-3</v>
       </c>
-      <c r="L7" s="92" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" s="92" t="s">
+      <c r="L7" s="91" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="91" t="s">
         <v>27</v>
       </c>
       <c r="N7" s="17">
         <v>0.35151719999999997</v>
       </c>
-      <c r="O7" s="92" t="s">
-        <v>27</v>
-      </c>
-      <c r="P7" s="92" t="s">
+      <c r="O7" s="91" t="s">
+        <v>27</v>
+      </c>
+      <c r="P7" s="91" t="s">
         <v>27</v>
       </c>
       <c r="Q7" s="5" t="s">
@@ -2193,7 +2235,7 @@
       <c r="H8" s="8">
         <v>1.4845112</v>
       </c>
-      <c r="I8" s="130">
+      <c r="I8" s="128">
         <v>0.14019999999999999</v>
       </c>
       <c r="J8" s="23">
@@ -2202,19 +2244,19 @@
       <c r="K8" s="8">
         <v>1.638595E-2</v>
       </c>
-      <c r="L8" s="93" t="s">
-        <v>27</v>
-      </c>
-      <c r="M8" s="93" t="s">
+      <c r="L8" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="92" t="s">
         <v>27</v>
       </c>
       <c r="N8" s="8">
         <v>0.27855829999999998</v>
       </c>
-      <c r="O8" s="93" t="s">
-        <v>27</v>
-      </c>
-      <c r="P8" s="93" t="s">
+      <c r="O8" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="P8" s="92" t="s">
         <v>27</v>
       </c>
       <c r="Q8" s="6" t="s">
@@ -2261,13 +2303,13 @@
       <c r="M9" s="26">
         <v>-1.92E-3</v>
       </c>
-      <c r="N9" s="98" t="s">
-        <v>27</v>
-      </c>
-      <c r="O9" s="98">
+      <c r="N9" s="97" t="s">
+        <v>27</v>
+      </c>
+      <c r="O9" s="97">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="P9" s="98" t="s">
+      <c r="P9" s="97" t="s">
         <v>27</v>
       </c>
       <c r="Q9" s="9" t="s">
@@ -2284,13 +2326,13 @@
       <c r="C10" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="88" t="s">
+      <c r="D10" s="87" t="s">
         <v>32</v>
       </c>
       <c r="E10" s="79">
         <v>129</v>
       </c>
-      <c r="F10" s="99">
+      <c r="F10" s="98">
         <v>0.23899999999999999</v>
       </c>
       <c r="G10" s="82">
@@ -2299,32 +2341,32 @@
       <c r="H10" s="82">
         <v>1.1830000000000001</v>
       </c>
-      <c r="I10" s="131">
+      <c r="I10" s="129">
         <v>0.23699999999999999</v>
       </c>
-      <c r="J10" s="99">
+      <c r="J10" s="98">
         <v>-9.9400000000000002E-2</v>
       </c>
       <c r="K10" s="82">
         <v>0.55800000000000005</v>
       </c>
-      <c r="L10" s="100" t="s">
-        <v>27</v>
-      </c>
-      <c r="M10" s="100" t="s">
-        <v>27</v>
-      </c>
-      <c r="N10" s="100" t="s">
-        <v>27</v>
-      </c>
-      <c r="O10" s="95">
+      <c r="L10" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="O10" s="94">
         <v>0.55700000000000005</v>
       </c>
-      <c r="P10" s="95">
+      <c r="P10" s="94">
         <v>1.244</v>
       </c>
       <c r="Q10" s="79" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
@@ -2364,19 +2406,19 @@
       <c r="K12" s="22">
         <v>2.3622690000000002E-3</v>
       </c>
-      <c r="L12" s="92" t="s">
+      <c r="L12" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="M12" s="92" t="s">
+      <c r="M12" s="91" t="s">
         <v>41</v>
       </c>
       <c r="N12" s="17">
         <v>0.35064200000000001</v>
       </c>
-      <c r="O12" s="92" t="s">
-        <v>27</v>
-      </c>
-      <c r="P12" s="92" t="s">
+      <c r="O12" s="91" t="s">
+        <v>27</v>
+      </c>
+      <c r="P12" s="91" t="s">
         <v>27</v>
       </c>
       <c r="Q12" s="5" t="s">
@@ -2418,19 +2460,19 @@
       <c r="K13" s="23">
         <v>1.051412E-2</v>
       </c>
-      <c r="L13" s="93" t="s">
-        <v>27</v>
-      </c>
-      <c r="M13" s="93" t="s">
+      <c r="L13" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="M13" s="92" t="s">
         <v>27</v>
       </c>
       <c r="N13" s="8">
         <v>0.29122520000000002</v>
       </c>
-      <c r="O13" s="93" t="s">
-        <v>27</v>
-      </c>
-      <c r="P13" s="93" t="s">
+      <c r="O13" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="P13" s="92" t="s">
         <v>27</v>
       </c>
       <c r="Q13" s="6" t="s">
@@ -2462,7 +2504,7 @@
       <c r="H14" s="19">
         <v>-1.4541999999999999</v>
       </c>
-      <c r="I14" s="90">
+      <c r="I14" s="89">
         <v>0.1484</v>
       </c>
       <c r="J14" s="26">
@@ -2477,13 +2519,13 @@
       <c r="M14" s="26">
         <v>2.5969999999999999E-3</v>
       </c>
-      <c r="N14" s="98" t="s">
-        <v>27</v>
-      </c>
-      <c r="O14" s="98">
+      <c r="N14" s="97" t="s">
+        <v>27</v>
+      </c>
+      <c r="O14" s="97">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="P14" s="98" t="s">
+      <c r="P14" s="97" t="s">
         <v>27</v>
       </c>
       <c r="Q14" s="9" t="s">
@@ -2500,7 +2542,7 @@
       <c r="C15" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="88" t="s">
+      <c r="D15" s="87" t="s">
         <v>21</v>
       </c>
       <c r="E15" s="79">
@@ -2515,22 +2557,22 @@
       <c r="H15" s="82">
         <v>-1.85</v>
       </c>
-      <c r="I15" s="132">
+      <c r="I15" s="130">
         <v>6.4299999999999996E-2</v>
       </c>
-      <c r="J15" s="99">
+      <c r="J15" s="98">
         <v>-1.0293000000000001</v>
       </c>
-      <c r="K15" s="99">
+      <c r="K15" s="98">
         <v>-0.13500000000000001</v>
       </c>
-      <c r="L15" s="100" t="s">
-        <v>27</v>
-      </c>
-      <c r="M15" s="100" t="s">
-        <v>27</v>
-      </c>
-      <c r="N15" s="100" t="s">
+      <c r="L15" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="N15" s="99" t="s">
         <v>27</v>
       </c>
       <c r="O15" s="82">
@@ -2540,7 +2582,7 @@
         <v>6.3179999999999996</v>
       </c>
       <c r="Q15" s="79" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.35">
@@ -2577,19 +2619,19 @@
       <c r="K17" s="22">
         <v>5.2589309999999997E-3</v>
       </c>
-      <c r="L17" s="92" t="s">
+      <c r="L17" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="M17" s="92" t="s">
+      <c r="M17" s="91" t="s">
         <v>41</v>
       </c>
       <c r="N17" s="17">
         <v>0.34664660000000003</v>
       </c>
-      <c r="O17" s="92" t="s">
-        <v>27</v>
-      </c>
-      <c r="P17" s="92" t="s">
+      <c r="O17" s="91" t="s">
+        <v>27</v>
+      </c>
+      <c r="P17" s="91" t="s">
         <v>27</v>
       </c>
       <c r="Q17" s="5" t="s">
@@ -2630,19 +2672,19 @@
       <c r="K18" s="8">
         <v>5.3303730000000001E-2</v>
       </c>
-      <c r="L18" s="93" t="s">
-        <v>27</v>
-      </c>
-      <c r="M18" s="93" t="s">
+      <c r="L18" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="M18" s="92" t="s">
         <v>27</v>
       </c>
       <c r="N18" s="8">
         <v>0.26359830000000001</v>
       </c>
-      <c r="O18" s="93" t="s">
-        <v>27</v>
-      </c>
-      <c r="P18" s="93" t="s">
+      <c r="O18" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="P18" s="92" t="s">
         <v>27</v>
       </c>
       <c r="Q18" s="6" t="s">
@@ -2680,7 +2722,7 @@
       <c r="J19" s="26">
         <v>-7.9984940000000001E-3</v>
       </c>
-      <c r="K19" s="107">
+      <c r="K19" s="106">
         <v>1.1316430000000001E-2</v>
       </c>
       <c r="L19" s="26">
@@ -2689,13 +2731,13 @@
       <c r="M19" s="19">
         <v>-1.323E-2</v>
       </c>
-      <c r="N19" s="98" t="s">
-        <v>27</v>
-      </c>
-      <c r="O19" s="98">
+      <c r="N19" s="97" t="s">
+        <v>27</v>
+      </c>
+      <c r="O19" s="97">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="P19" s="98" t="s">
+      <c r="P19" s="97" t="s">
         <v>27</v>
       </c>
       <c r="Q19" s="9" t="s">
@@ -2712,7 +2754,7 @@
       <c r="C20" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="88" t="s">
+      <c r="D20" s="87" t="s">
         <v>33</v>
       </c>
       <c r="E20" s="79">
@@ -2727,7 +2769,7 @@
       <c r="H20" s="82">
         <v>1.1359999999999999</v>
       </c>
-      <c r="I20" s="91">
+      <c r="I20" s="90">
         <v>0.25600000000000001</v>
       </c>
       <c r="J20" s="82">
@@ -2736,13 +2778,13 @@
       <c r="K20" s="82">
         <v>0.63700000000000001</v>
       </c>
-      <c r="L20" s="95" t="s">
-        <v>27</v>
-      </c>
-      <c r="M20" s="95" t="s">
-        <v>27</v>
-      </c>
-      <c r="N20" s="95" t="s">
+      <c r="L20" s="94" t="s">
+        <v>27</v>
+      </c>
+      <c r="M20" s="94" t="s">
+        <v>27</v>
+      </c>
+      <c r="N20" s="94" t="s">
         <v>27</v>
       </c>
       <c r="O20" s="82">
@@ -2752,7 +2794,7 @@
         <v>7.6319999999999997</v>
       </c>
       <c r="Q20" s="79" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2765,10 +2807,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB8E188F-C842-439D-93EC-074F9278CAC0}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="Q8" sqref="Q8"/>
+      <selection pane="bottomLeft" activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2837,7 +2879,7 @@
       <c r="P1" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="110" t="s">
+      <c r="Q1" s="109" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2875,19 +2917,19 @@
       <c r="K2" s="22">
         <v>-8.8493200000000008E-3</v>
       </c>
-      <c r="L2" s="92" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="92" t="s">
+      <c r="L2" s="91" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="91" t="s">
         <v>27</v>
       </c>
       <c r="N2" s="17">
         <v>0.41643530000000001</v>
       </c>
-      <c r="O2" s="96" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="96" t="s">
+      <c r="O2" s="95" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="95" t="s">
         <v>27</v>
       </c>
       <c r="Q2" s="5" t="s">
@@ -2928,19 +2970,19 @@
       <c r="K3" s="8">
         <v>0.39153739999999998</v>
       </c>
-      <c r="L3" s="93" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="93" t="s">
+      <c r="L3" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="92" t="s">
         <v>27</v>
       </c>
       <c r="N3" s="8">
         <v>0.25423780000000001</v>
       </c>
-      <c r="O3" s="97" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" s="97" t="s">
+      <c r="O3" s="96" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" s="96" t="s">
         <v>27</v>
       </c>
       <c r="Q3" s="6" t="s">
@@ -2987,13 +3029,13 @@
       <c r="M4" s="19">
         <v>-1.456E-2</v>
       </c>
-      <c r="N4" s="94" t="s">
+      <c r="N4" s="93" t="s">
         <v>27</v>
       </c>
       <c r="O4" s="19">
         <v>6.9250500000000006E-2</v>
       </c>
-      <c r="P4" s="98" t="s">
+      <c r="P4" s="97" t="s">
         <v>27</v>
       </c>
       <c r="Q4" s="9" t="s">
@@ -3016,16 +3058,16 @@
       <c r="E5" s="79">
         <v>102</v>
       </c>
-      <c r="F5" s="99">
+      <c r="F5" s="98">
         <v>1.8200000000000001E-2</v>
       </c>
       <c r="G5" s="82">
         <v>0.28399999999999997</v>
       </c>
-      <c r="H5" s="99">
+      <c r="H5" s="98">
         <v>6.3899999999999998E-2</v>
       </c>
-      <c r="I5" s="91">
+      <c r="I5" s="90">
         <v>0.94899999999999995</v>
       </c>
       <c r="J5" s="82">
@@ -3034,13 +3076,13 @@
       <c r="K5" s="82">
         <v>0.75600000000000001</v>
       </c>
-      <c r="L5" s="95" t="s">
-        <v>27</v>
-      </c>
-      <c r="M5" s="95" t="s">
-        <v>27</v>
-      </c>
-      <c r="N5" s="95" t="s">
+      <c r="L5" s="94" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="94" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="94" t="s">
         <v>27</v>
       </c>
       <c r="O5" s="82">
@@ -3050,7 +3092,7 @@
         <v>1.25</v>
       </c>
       <c r="Q5" s="79" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
@@ -3090,19 +3132,19 @@
       <c r="K7" s="17">
         <v>7.9127550000000005E-2</v>
       </c>
-      <c r="L7" s="92" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" s="92" t="s">
+      <c r="L7" s="91" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="91" t="s">
         <v>27</v>
       </c>
       <c r="N7" s="17">
         <v>0.31013429999999997</v>
       </c>
-      <c r="O7" s="92" t="s">
-        <v>27</v>
-      </c>
-      <c r="P7" s="92" t="s">
+      <c r="O7" s="91" t="s">
+        <v>27</v>
+      </c>
+      <c r="P7" s="91" t="s">
         <v>27</v>
       </c>
       <c r="Q7" s="5" t="s">
@@ -3143,19 +3185,19 @@
       <c r="K8" s="8">
         <v>0.23089009999999999</v>
       </c>
-      <c r="L8" s="93" t="s">
-        <v>27</v>
-      </c>
-      <c r="M8" s="93" t="s">
+      <c r="L8" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="92" t="s">
         <v>27</v>
       </c>
       <c r="N8" s="8">
         <v>0.37893369999999998</v>
       </c>
-      <c r="O8" s="93" t="s">
-        <v>27</v>
-      </c>
-      <c r="P8" s="93" t="s">
+      <c r="O8" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="P8" s="92" t="s">
         <v>27</v>
       </c>
       <c r="Q8" s="6" t="s">
@@ -3202,13 +3244,13 @@
       <c r="M9" s="26">
         <v>-5.2469999999999999E-3</v>
       </c>
-      <c r="N9" s="94" t="s">
+      <c r="N9" s="93" t="s">
         <v>27</v>
       </c>
       <c r="O9" s="26">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="P9" s="98" t="s">
+      <c r="P9" s="97" t="s">
         <v>27</v>
       </c>
       <c r="Q9" s="9" t="s">
@@ -3240,7 +3282,7 @@
       <c r="H10" s="82">
         <v>-0.92100000000000004</v>
       </c>
-      <c r="I10" s="91">
+      <c r="I10" s="90">
         <v>0.35699999999999998</v>
       </c>
       <c r="J10" s="82">
@@ -3249,13 +3291,13 @@
       <c r="K10" s="82">
         <v>0.185</v>
       </c>
-      <c r="L10" s="95" t="s">
-        <v>27</v>
-      </c>
-      <c r="M10" s="95" t="s">
-        <v>27</v>
-      </c>
-      <c r="N10" s="95" t="s">
+      <c r="L10" s="94" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="94" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" s="94" t="s">
         <v>27</v>
       </c>
       <c r="O10" s="82">
@@ -3265,7 +3307,7 @@
         <v>1.244</v>
       </c>
       <c r="Q10" s="79" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
@@ -3305,19 +3347,19 @@
       <c r="K12" s="22">
         <v>3.6737900000000001E-3</v>
       </c>
-      <c r="L12" s="92" t="s">
-        <v>27</v>
-      </c>
-      <c r="M12" s="92" t="s">
+      <c r="L12" s="91" t="s">
+        <v>27</v>
+      </c>
+      <c r="M12" s="91" t="s">
         <v>27</v>
       </c>
       <c r="N12" s="17">
         <v>0.30335590000000001</v>
       </c>
-      <c r="O12" s="92" t="s">
-        <v>27</v>
-      </c>
-      <c r="P12" s="92" t="s">
+      <c r="O12" s="91" t="s">
+        <v>27</v>
+      </c>
+      <c r="P12" s="91" t="s">
         <v>27</v>
       </c>
       <c r="Q12" s="5" t="s">
@@ -3358,19 +3400,19 @@
       <c r="K13" s="8">
         <v>3.7587820000000001E-2</v>
       </c>
-      <c r="L13" s="93" t="s">
-        <v>27</v>
-      </c>
-      <c r="M13" s="93" t="s">
+      <c r="L13" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="M13" s="92" t="s">
         <v>27</v>
       </c>
       <c r="N13" s="8">
         <v>0.29893370000000002</v>
       </c>
-      <c r="O13" s="93" t="s">
-        <v>27</v>
-      </c>
-      <c r="P13" s="93" t="s">
+      <c r="O13" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="P13" s="92" t="s">
         <v>27</v>
       </c>
       <c r="Q13" s="6" t="s">
@@ -3417,13 +3459,13 @@
       <c r="M14" s="26">
         <v>-1.376E-2</v>
       </c>
-      <c r="N14" s="94" t="s">
+      <c r="N14" s="93" t="s">
         <v>27</v>
       </c>
       <c r="O14" s="26">
         <v>1.081113E-7</v>
       </c>
-      <c r="P14" s="98" t="s">
+      <c r="P14" s="97" t="s">
         <v>27</v>
       </c>
       <c r="Q14" s="9" t="s">
@@ -3455,7 +3497,7 @@
       <c r="H15" s="82">
         <v>-0.316</v>
       </c>
-      <c r="I15" s="91">
+      <c r="I15" s="90">
         <v>0.752</v>
       </c>
       <c r="J15" s="82">
@@ -3464,13 +3506,13 @@
       <c r="K15" s="82">
         <v>0.434</v>
       </c>
-      <c r="L15" s="95" t="s">
-        <v>27</v>
-      </c>
-      <c r="M15" s="95" t="s">
-        <v>27</v>
-      </c>
-      <c r="N15" s="95" t="s">
+      <c r="L15" s="94" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="94" t="s">
+        <v>27</v>
+      </c>
+      <c r="N15" s="94" t="s">
         <v>27</v>
       </c>
       <c r="O15" s="82">
@@ -3480,7 +3522,7 @@
         <v>1.2390000000000001</v>
       </c>
       <c r="Q15" s="79" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.35">
@@ -3517,19 +3559,19 @@
       <c r="K17" s="17">
         <v>0.25631401199999998</v>
       </c>
-      <c r="L17" s="92" t="s">
-        <v>27</v>
-      </c>
-      <c r="M17" s="92" t="s">
+      <c r="L17" s="91" t="s">
+        <v>27</v>
+      </c>
+      <c r="M17" s="91" t="s">
         <v>27</v>
       </c>
       <c r="N17" s="17">
         <v>0.38511570000000001</v>
       </c>
-      <c r="O17" s="92" t="s">
-        <v>27</v>
-      </c>
-      <c r="P17" s="92" t="s">
+      <c r="O17" s="91" t="s">
+        <v>27</v>
+      </c>
+      <c r="P17" s="91" t="s">
         <v>27</v>
       </c>
       <c r="Q17" s="5" t="s">
@@ -3570,19 +3612,19 @@
       <c r="K18" s="8">
         <v>1.6610862</v>
       </c>
-      <c r="L18" s="93" t="s">
-        <v>27</v>
-      </c>
-      <c r="M18" s="93" t="s">
+      <c r="L18" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="M18" s="92" t="s">
         <v>27</v>
       </c>
       <c r="N18" s="8">
         <v>0.25619589999999998</v>
       </c>
-      <c r="O18" s="93" t="s">
-        <v>27</v>
-      </c>
-      <c r="P18" s="93" t="s">
+      <c r="O18" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="P18" s="92" t="s">
         <v>27</v>
       </c>
       <c r="Q18" s="6" t="s">
@@ -3614,7 +3656,7 @@
       <c r="H19" s="19">
         <v>1.5656000000000001</v>
       </c>
-      <c r="I19" s="90">
+      <c r="I19" s="89">
         <v>0.11990000000000001</v>
       </c>
       <c r="J19" s="19">
@@ -3629,13 +3671,13 @@
       <c r="M19" s="19">
         <v>5.2100000000000002E-3</v>
       </c>
-      <c r="N19" s="94" t="s">
+      <c r="N19" s="93" t="s">
         <v>27</v>
       </c>
       <c r="O19" s="19">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="P19" s="98" t="s">
+      <c r="P19" s="97" t="s">
         <v>27</v>
       </c>
       <c r="Q19" s="9" t="s">
@@ -3667,22 +3709,22 @@
       <c r="H20" s="82">
         <v>1.534</v>
       </c>
-      <c r="I20" s="118">
+      <c r="I20" s="117">
         <v>0.125</v>
       </c>
-      <c r="J20" s="134">
+      <c r="J20" s="132">
         <v>0.186</v>
       </c>
-      <c r="K20" s="134">
+      <c r="K20" s="132">
         <v>0.56000000000000005</v>
       </c>
-      <c r="L20" s="95" t="s">
-        <v>27</v>
-      </c>
-      <c r="M20" s="95" t="s">
-        <v>27</v>
-      </c>
-      <c r="N20" s="95" t="s">
+      <c r="L20" s="94" t="s">
+        <v>27</v>
+      </c>
+      <c r="M20" s="94" t="s">
+        <v>27</v>
+      </c>
+      <c r="N20" s="94" t="s">
         <v>27</v>
       </c>
       <c r="O20" s="82">
@@ -3692,12 +3734,12 @@
         <v>1.2390000000000001</v>
       </c>
       <c r="Q20" s="79" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="Q21" s="75" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -3707,11 +3749,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA225CA-067B-4F77-85FD-EE40FC6CFFCC}">
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3811,19 +3853,19 @@
       <c r="K2" s="22">
         <v>-7.2038249999999996E-3</v>
       </c>
-      <c r="L2" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="103" t="s">
+      <c r="L2" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="102" t="s">
         <v>27</v>
       </c>
       <c r="N2" s="5">
         <v>0.31788480000000002</v>
       </c>
-      <c r="O2" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="103" t="s">
+      <c r="O2" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="102" t="s">
         <v>27</v>
       </c>
       <c r="Q2" s="5" t="s">
@@ -3864,19 +3906,19 @@
       <c r="K3" s="8">
         <v>5.6547790000000001E-2</v>
       </c>
-      <c r="L3" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="104" t="s">
+      <c r="L3" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="103" t="s">
         <v>27</v>
       </c>
       <c r="N3" s="6">
         <v>0.1613368</v>
       </c>
-      <c r="O3" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" s="104" t="s">
+      <c r="O3" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" s="103" t="s">
         <v>27</v>
       </c>
       <c r="Q3" s="6" t="s">
@@ -3923,13 +3965,13 @@
       <c r="M4" s="9">
         <v>-1.0670000000000001E-2</v>
       </c>
-      <c r="N4" s="106" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" s="106">
+      <c r="N4" s="105" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" s="105">
         <v>2.2109679999999998E-3</v>
       </c>
-      <c r="P4" s="106" t="s">
+      <c r="P4" s="105" t="s">
         <v>27</v>
       </c>
       <c r="Q4" s="9" t="s">
@@ -3952,23 +3994,42 @@
       <c r="E5" s="79">
         <v>129</v>
       </c>
-      <c r="F5" s="82"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="82"/>
-      <c r="I5" s="82"/>
-      <c r="J5" s="82"/>
-      <c r="K5" s="82"/>
-      <c r="L5" s="105" t="s">
-        <v>27</v>
-      </c>
-      <c r="M5" s="105" t="s">
-        <v>27</v>
-      </c>
-      <c r="N5" s="105" t="s">
-        <v>27</v>
-      </c>
-      <c r="O5" s="82"/>
-      <c r="P5" s="82"/>
+      <c r="F5" s="82">
+        <v>-0.318</v>
+      </c>
+      <c r="G5" s="82">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="H5" s="82">
+        <v>-0.65200000000000002</v>
+      </c>
+      <c r="I5" s="82">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="J5" s="82">
+        <v>-1.165</v>
+      </c>
+      <c r="K5" s="82">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="L5" s="104" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="104" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="104" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5" s="82">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="P5" s="82">
+        <v>1.2390000000000001</v>
+      </c>
+      <c r="Q5" s="79" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="13"/>
@@ -4011,19 +4072,19 @@
       <c r="K7" s="63">
         <v>-9.0268349999999997E-2</v>
       </c>
-      <c r="L7" s="111" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" s="111" t="s">
+      <c r="L7" s="110" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="110" t="s">
         <v>27</v>
       </c>
       <c r="N7" s="63">
         <v>0.14573320000000001</v>
       </c>
-      <c r="O7" s="111" t="s">
-        <v>27</v>
-      </c>
-      <c r="P7" s="111" t="s">
+      <c r="O7" s="110" t="s">
+        <v>27</v>
+      </c>
+      <c r="P7" s="110" t="s">
         <v>27</v>
       </c>
       <c r="Q7" s="65" t="s">
@@ -4064,19 +4125,19 @@
       <c r="K8" s="59">
         <v>-3.5458910000000003E-2</v>
       </c>
-      <c r="L8" s="112" t="s">
-        <v>27</v>
-      </c>
-      <c r="M8" s="112" t="s">
+      <c r="L8" s="111" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="111" t="s">
         <v>27</v>
       </c>
       <c r="N8" s="59">
         <v>0.3</v>
       </c>
-      <c r="O8" s="112" t="s">
-        <v>27</v>
-      </c>
-      <c r="P8" s="112" t="s">
+      <c r="O8" s="111" t="s">
+        <v>27</v>
+      </c>
+      <c r="P8" s="111" t="s">
         <v>27</v>
       </c>
       <c r="Q8" s="67" t="s">
@@ -4123,13 +4184,13 @@
       <c r="M9" s="69">
         <v>-7.77E-3</v>
       </c>
-      <c r="N9" s="113" t="s">
-        <v>27</v>
-      </c>
-      <c r="O9" s="113">
+      <c r="N9" s="112" t="s">
+        <v>27</v>
+      </c>
+      <c r="O9" s="112">
         <v>2.036871E-3</v>
       </c>
-      <c r="P9" s="113" t="s">
+      <c r="P9" s="112" t="s">
         <v>27</v>
       </c>
       <c r="Q9" s="71" t="s">
@@ -4149,831 +4210,925 @@
       <c r="D10" s="77" t="s">
         <v>97</v>
       </c>
-      <c r="E10" s="133">
+      <c r="E10" s="131">
         <v>104</v>
       </c>
-      <c r="F10" s="83"/>
-      <c r="G10" s="83"/>
-      <c r="H10" s="83"/>
-      <c r="I10" s="120"/>
-      <c r="J10" s="83"/>
-      <c r="K10" s="83"/>
-      <c r="L10" s="114" t="s">
-        <v>27</v>
-      </c>
-      <c r="M10" s="114" t="s">
-        <v>27</v>
-      </c>
-      <c r="N10" s="114" t="s">
-        <v>27</v>
-      </c>
-      <c r="O10" s="119"/>
-      <c r="P10" s="83"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A11" s="13"/>
-    </row>
-    <row r="12" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
+      <c r="F10" s="83">
+        <v>-1.0371999999999999</v>
+      </c>
+      <c r="G10" s="83">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="H10" s="83">
+        <v>-2.0064700000000002</v>
+      </c>
+      <c r="I10" s="134">
+        <v>4.48E-2</v>
+      </c>
+      <c r="J10" s="83">
+        <v>-2.2650000000000001</v>
+      </c>
+      <c r="K10" s="83">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="L10" s="113" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="113" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" s="113" t="s">
+        <v>27</v>
+      </c>
+      <c r="O10" s="118">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="P10" s="83">
+        <v>1.246</v>
+      </c>
+      <c r="Q10" s="77" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" s="136" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="135"/>
+      <c r="E11" s="137"/>
+      <c r="F11" s="138"/>
+      <c r="G11" s="138"/>
+      <c r="H11" s="138"/>
+      <c r="I11" s="139"/>
+      <c r="J11" s="133">
+        <v>2.07E-2</v>
+      </c>
+      <c r="K11" s="133">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="L11" s="140"/>
+      <c r="M11" s="140"/>
+      <c r="N11" s="140"/>
+      <c r="O11" s="141"/>
+      <c r="P11" s="138"/>
+      <c r="Q11" s="75" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" s="13"/>
+    </row>
+    <row r="13" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E13" s="5">
         <v>796</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F13" s="17">
         <v>0.17676629999999999</v>
       </c>
-      <c r="G12" s="17">
+      <c r="G13" s="17">
         <v>5.066615E-2</v>
       </c>
-      <c r="H12" s="17">
+      <c r="H13" s="17">
         <v>3.4888439999999998</v>
       </c>
-      <c r="I12" s="58">
+      <c r="I13" s="58">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="J12" s="17">
+      <c r="J13" s="17">
         <v>7.7462470000000005E-2</v>
       </c>
-      <c r="K12" s="17">
+      <c r="K13" s="17">
         <v>0.27607010999999998</v>
       </c>
-      <c r="L12" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="M12" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="N12" s="5">
+      <c r="L13" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="M13" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="N13" s="5">
         <v>0.32124799999999998</v>
       </c>
-      <c r="O12" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="P12" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q12" s="5" t="s">
+      <c r="O13" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="P13" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q13" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
+    <row r="14" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E14" s="6">
         <v>130</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F14" s="8">
         <v>0.37727919999999998</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G14" s="8">
         <v>0.26005499999999998</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H14" s="8">
         <v>1.4507669999999999</v>
       </c>
-      <c r="I13" s="33">
+      <c r="I14" s="33">
         <v>0.14929999999999999</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J14" s="8">
         <v>-0.13241919999999999</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K14" s="8">
         <v>0.88697769999999998</v>
       </c>
-      <c r="L13" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="M13" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="N13" s="6">
+      <c r="L14" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="M14" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14" s="6">
         <v>0.19552069999999999</v>
       </c>
-      <c r="O13" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="P13" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q13" s="6" t="s">
+      <c r="O14" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="P14" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q14" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="12" t="s">
+    <row r="15" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C15" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D15" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E15" s="9">
         <v>129</v>
       </c>
-      <c r="F14" s="19">
+      <c r="F15" s="19">
         <v>0.18750500000000001</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G15" s="19">
         <v>8.6096000000000006E-2</v>
       </c>
-      <c r="H14" s="19">
+      <c r="H15" s="19">
         <v>2.1779000000000002</v>
       </c>
-      <c r="I14" s="36">
+      <c r="I15" s="36">
         <v>3.1280000000000002E-2</v>
       </c>
-      <c r="J14" s="19">
+      <c r="J15" s="19">
         <v>1.8760120000000002E-2</v>
       </c>
-      <c r="K14" s="19">
+      <c r="K15" s="19">
         <v>0.3562496</v>
       </c>
-      <c r="L14" s="9" t="s">
+      <c r="L15" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="M14" s="9">
+      <c r="M15" s="9">
         <v>2.265E-2</v>
       </c>
-      <c r="N14" s="106" t="s">
-        <v>27</v>
-      </c>
-      <c r="O14" s="106">
+      <c r="N15" s="105" t="s">
+        <v>27</v>
+      </c>
+      <c r="O15" s="105">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="P14" s="106" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q14" s="9" t="s">
+      <c r="P15" s="105" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q15" s="9" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="79" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="78" t="s">
+    <row r="16" spans="1:17" s="79" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="79" t="s">
+      <c r="B16" s="79" t="s">
         <v>112</v>
       </c>
-      <c r="C15" s="79" t="s">
+      <c r="C16" s="79" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="79" t="s">
+      <c r="D16" s="79" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="79">
+      <c r="E16" s="79">
         <v>129</v>
       </c>
-      <c r="F15" s="82"/>
-      <c r="G15" s="82"/>
-      <c r="H15" s="82"/>
-      <c r="I15" s="85"/>
-      <c r="J15" s="82"/>
-      <c r="K15" s="82"/>
-      <c r="L15" s="105" t="s">
-        <v>27</v>
-      </c>
-      <c r="M15" s="105" t="s">
-        <v>27</v>
-      </c>
-      <c r="N15" s="105" t="s">
-        <v>27</v>
-      </c>
-      <c r="O15" s="82"/>
-      <c r="P15" s="82"/>
-    </row>
-    <row r="16" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="13"/>
-      <c r="I16" s="53"/>
-      <c r="N16" s="54"/>
-      <c r="O16" s="54"/>
-      <c r="P16" s="54"/>
-    </row>
-    <row r="17" spans="1:17" s="62" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="61" t="s">
+      <c r="F16" s="82">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="G16" s="82">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="H16" s="82">
+        <v>2.1850000000000001</v>
+      </c>
+      <c r="I16" s="84">
+        <v>2.8899999999999999E-2</v>
+      </c>
+      <c r="J16" s="82">
+        <v>0.18</v>
+      </c>
+      <c r="K16" s="82">
+        <v>1.6890000000000001</v>
+      </c>
+      <c r="L16" s="104" t="s">
+        <v>27</v>
+      </c>
+      <c r="M16" s="104" t="s">
+        <v>27</v>
+      </c>
+      <c r="N16" s="104" t="s">
+        <v>27</v>
+      </c>
+      <c r="O16" s="82">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="P16" s="82">
+        <v>1.278</v>
+      </c>
+      <c r="Q16" s="79" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="13"/>
+      <c r="I17" s="53"/>
+      <c r="N17" s="54"/>
+      <c r="O17" s="54"/>
+      <c r="P17" s="54"/>
+    </row>
+    <row r="18" spans="1:17" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="62" t="s">
+      <c r="B18" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="62" t="s">
+      <c r="C18" s="62" t="s">
         <v>94</v>
       </c>
-      <c r="D17" s="62" t="s">
+      <c r="D18" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="E17" s="62">
+      <c r="E18" s="62">
         <v>575</v>
       </c>
-      <c r="F17" s="63">
+      <c r="F18" s="63">
         <v>0.214503</v>
       </c>
-      <c r="G17" s="63">
+      <c r="G18" s="63">
         <v>6.7277190000000001E-2</v>
       </c>
-      <c r="H17" s="63">
+      <c r="H18" s="63">
         <v>3.1883469999999998</v>
       </c>
-      <c r="I17" s="72">
+      <c r="I18" s="72">
         <v>1.5E-3</v>
       </c>
-      <c r="J17" s="63">
+      <c r="J18" s="63">
         <v>8.2642160000000006E-2</v>
       </c>
-      <c r="K17" s="63">
+      <c r="K18" s="63">
         <v>0.3463639</v>
       </c>
-      <c r="L17" s="111" t="s">
-        <v>27</v>
-      </c>
-      <c r="M17" s="111" t="s">
-        <v>27</v>
-      </c>
-      <c r="N17" s="73">
+      <c r="L18" s="110" t="s">
+        <v>27</v>
+      </c>
+      <c r="M18" s="110" t="s">
+        <v>27</v>
+      </c>
+      <c r="N18" s="73">
         <v>0.1434502</v>
       </c>
-      <c r="O17" s="111" t="s">
-        <v>27</v>
-      </c>
-      <c r="P17" s="111" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q17" s="62" t="s">
+      <c r="O18" s="110" t="s">
+        <v>27</v>
+      </c>
+      <c r="P18" s="110" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q18" s="62" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="56" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="66" t="s">
+    <row r="19" spans="1:17" s="56" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="56" t="s">
+      <c r="B19" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="56" t="s">
+      <c r="C19" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="D18" s="56" t="s">
+      <c r="D19" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="E18" s="56">
+      <c r="E19" s="56">
         <v>91</v>
       </c>
-      <c r="F18" s="59">
+      <c r="F19" s="59">
         <v>0.72873929999999998</v>
       </c>
-      <c r="G18" s="59">
+      <c r="G19" s="59">
         <v>0.35372100000000001</v>
       </c>
-      <c r="H18" s="59">
+      <c r="H19" s="59">
         <v>2.060209</v>
       </c>
-      <c r="I18" s="60">
+      <c r="I19" s="60">
         <v>4.2299999999999997E-2</v>
       </c>
-      <c r="J18" s="59">
+      <c r="J19" s="59">
         <v>3.5458910000000003E-2</v>
       </c>
-      <c r="K18" s="59">
+      <c r="K19" s="59">
         <v>1.4220197000000001</v>
       </c>
-      <c r="L18" s="112" t="s">
-        <v>27</v>
-      </c>
-      <c r="M18" s="112" t="s">
-        <v>27</v>
-      </c>
-      <c r="N18" s="74">
+      <c r="L19" s="111" t="s">
+        <v>27</v>
+      </c>
+      <c r="M19" s="111" t="s">
+        <v>27</v>
+      </c>
+      <c r="N19" s="74">
         <v>0.3</v>
       </c>
-      <c r="O18" s="112" t="s">
-        <v>27</v>
-      </c>
-      <c r="P18" s="112" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q18" s="56" t="s">
+      <c r="O19" s="111" t="s">
+        <v>27</v>
+      </c>
+      <c r="P19" s="111" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q19" s="56" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="69" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="68" t="s">
+    <row r="20" spans="1:17" s="69" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="69" t="s">
+      <c r="B20" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="69" t="s">
+      <c r="C20" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="D19" s="69" t="s">
+      <c r="D20" s="69" t="s">
         <v>99</v>
       </c>
-      <c r="E19" s="69">
+      <c r="E20" s="69">
         <v>104</v>
       </c>
-      <c r="F19" s="70">
+      <c r="F20" s="70">
         <v>0.120382</v>
       </c>
-      <c r="G19" s="70">
+      <c r="G20" s="70">
         <v>0.109667</v>
       </c>
-      <c r="H19" s="70">
+      <c r="H20" s="70">
         <v>1.0976999999999999</v>
       </c>
-      <c r="I19" s="70">
+      <c r="I20" s="70">
         <v>0.27489999999999998</v>
       </c>
-      <c r="J19" s="70">
+      <c r="J20" s="70">
         <v>-9.4561439999999997E-2</v>
       </c>
-      <c r="K19" s="70">
+      <c r="K20" s="70">
         <v>0.33532611000000001</v>
       </c>
-      <c r="L19" s="69" t="s">
+      <c r="L20" s="69" t="s">
         <v>104</v>
       </c>
-      <c r="M19" s="69">
+      <c r="M20" s="69">
         <v>7.77E-3</v>
       </c>
-      <c r="N19" s="113" t="s">
-        <v>27</v>
-      </c>
-      <c r="O19" s="113">
+      <c r="N20" s="112" t="s">
+        <v>27</v>
+      </c>
+      <c r="O20" s="112">
         <v>2.036871E-3</v>
       </c>
-      <c r="P19" s="113" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q19" s="69" t="s">
+      <c r="P20" s="112" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q20" s="69" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="77" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="76" t="s">
+    <row r="21" spans="1:17" s="77" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="77" t="s">
+      <c r="B21" s="77" t="s">
         <v>112</v>
       </c>
-      <c r="C20" s="77" t="s">
+      <c r="C21" s="77" t="s">
         <v>94</v>
       </c>
-      <c r="D20" s="77" t="s">
+      <c r="D21" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="E20" s="133">
+      <c r="E21" s="131">
         <v>104</v>
       </c>
-      <c r="F20" s="83"/>
-      <c r="G20" s="83"/>
-      <c r="H20" s="83"/>
-      <c r="I20" s="83"/>
-      <c r="J20" s="83"/>
-      <c r="K20" s="83"/>
-      <c r="L20" s="114" t="s">
-        <v>27</v>
-      </c>
-      <c r="M20" s="114" t="s">
-        <v>27</v>
-      </c>
-      <c r="N20" s="114" t="s">
-        <v>27</v>
-      </c>
-      <c r="O20" s="84"/>
-      <c r="P20" s="84"/>
-      <c r="Q20" s="133"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A21" s="13"/>
+      <c r="F21" s="83">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="G21" s="83">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="H21" s="83">
+        <v>1.8260000000000001</v>
+      </c>
+      <c r="I21" s="83">
+        <v>6.7799999999999999E-2</v>
+      </c>
+      <c r="J21" s="83">
+        <v>-0.41</v>
+      </c>
+      <c r="K21" s="83">
+        <v>2.0051999999999999</v>
+      </c>
+      <c r="L21" s="113" t="s">
+        <v>27</v>
+      </c>
+      <c r="M21" s="113" t="s">
+        <v>27</v>
+      </c>
+      <c r="N21" s="113" t="s">
+        <v>27</v>
+      </c>
+      <c r="O21" s="83">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="P21" s="83">
+        <v>1.2410000000000001</v>
+      </c>
+      <c r="Q21" s="131" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="13"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A23" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E23" s="5">
         <v>733</v>
       </c>
-      <c r="F22" s="17">
+      <c r="F23" s="17">
         <v>3.3735099999999997E-2</v>
       </c>
-      <c r="G22" s="17">
+      <c r="G23" s="17">
         <v>7.7621560000000006E-2</v>
       </c>
-      <c r="H22" s="17">
+      <c r="H23" s="17">
         <v>0.43460900000000002</v>
       </c>
-      <c r="I22" s="17">
+      <c r="I23" s="17">
         <v>0.66400000000000003</v>
       </c>
-      <c r="J22" s="17">
+      <c r="J23" s="17">
         <v>-0.11840041</v>
       </c>
-      <c r="K22" s="17">
+      <c r="K23" s="17">
         <v>0.18587053000000001</v>
       </c>
-      <c r="L22" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="M22" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="N22" s="17">
+      <c r="L23" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="M23" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="N23" s="17">
         <v>0.37230829999999998</v>
       </c>
-      <c r="O22" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="P22" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q22" s="5" t="s">
+      <c r="O23" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="P23" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q23" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A23" s="11" t="s">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A24" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B24" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C24" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D24" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E24" s="6">
         <v>117</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F24" s="8">
         <v>-0.21963659999999999</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G24" s="8">
         <v>0.49134080000000002</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H24" s="8">
         <v>-0.44701469999999999</v>
       </c>
-      <c r="I23" s="8">
+      <c r="I24" s="8">
         <v>0.65569999999999995</v>
       </c>
-      <c r="J23" s="8">
+      <c r="J24" s="8">
         <v>-1.1826467700000001</v>
       </c>
-      <c r="K23" s="8">
+      <c r="K24" s="8">
         <v>0.74337370000000003</v>
       </c>
-      <c r="L23" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="M23" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="N23" s="8">
+      <c r="L24" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="M24" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="N24" s="8">
         <v>0.3196425</v>
       </c>
-      <c r="O23" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="P23" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q23" s="6" t="s">
+      <c r="O24" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="P24" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q24" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A24" s="40" t="s">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A25" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="39" t="s">
+      <c r="B25" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="39" t="s">
+      <c r="C25" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="39" t="s">
+      <c r="D25" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="E24" s="39">
+      <c r="E25" s="39">
         <v>122</v>
       </c>
-      <c r="F24" s="41">
+      <c r="F25" s="41">
         <v>-0.247531</v>
       </c>
-      <c r="G24" s="41">
+      <c r="G25" s="41">
         <v>0.17519100000000001</v>
       </c>
-      <c r="H24" s="41">
+      <c r="H25" s="41">
         <v>-1.4129</v>
       </c>
-      <c r="I24" s="42">
+      <c r="I25" s="42">
         <v>0.16028999999999999</v>
       </c>
-      <c r="J24" s="41">
+      <c r="J25" s="41">
         <v>-0.59089959999999997</v>
       </c>
-      <c r="K24" s="41">
+      <c r="K25" s="41">
         <v>9.5837240000000004E-2</v>
       </c>
-      <c r="L24" s="39">
+      <c r="L25" s="39">
         <v>1.7909999999999999E-2</v>
       </c>
-      <c r="M24" s="39">
+      <c r="M25" s="39">
         <v>1.4090000000000001E-3</v>
       </c>
-      <c r="N24" s="106" t="s">
-        <v>27</v>
-      </c>
-      <c r="O24" s="115">
+      <c r="N25" s="105" t="s">
+        <v>27</v>
+      </c>
+      <c r="O25" s="114">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="P24" s="106" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q24" s="39" t="s">
+      <c r="P25" s="105" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q25" s="39" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="79" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="87" t="s">
+    <row r="26" spans="1:17" s="79" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="86" t="s">
+      <c r="B26" s="85" t="s">
         <v>112</v>
       </c>
-      <c r="C25" s="86" t="s">
+      <c r="C26" s="85" t="s">
         <v>94</v>
       </c>
-      <c r="D25" s="86" t="s">
+      <c r="D26" s="85" t="s">
         <v>54</v>
       </c>
-      <c r="E25" s="86">
+      <c r="E26" s="85">
         <v>122</v>
       </c>
-      <c r="F25" s="127" t="s">
-        <v>118</v>
-      </c>
-      <c r="G25" s="127" t="s">
-        <v>118</v>
-      </c>
-      <c r="H25" s="127" t="s">
-        <v>118</v>
-      </c>
-      <c r="I25" s="127" t="s">
-        <v>118</v>
-      </c>
-      <c r="J25" s="127" t="s">
-        <v>118</v>
-      </c>
-      <c r="K25" s="127" t="s">
-        <v>118</v>
-      </c>
-      <c r="L25" s="127" t="s">
-        <v>118</v>
-      </c>
-      <c r="M25" s="105" t="s">
-        <v>27</v>
-      </c>
-      <c r="N25" s="105" t="s">
-        <v>27</v>
-      </c>
-      <c r="O25" s="127" t="s">
-        <v>118</v>
-      </c>
-      <c r="P25" s="127" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q25" s="86" t="s">
+      <c r="F26" s="125" t="s">
+        <v>117</v>
+      </c>
+      <c r="G26" s="125" t="s">
+        <v>117</v>
+      </c>
+      <c r="H26" s="125" t="s">
+        <v>117</v>
+      </c>
+      <c r="I26" s="125" t="s">
+        <v>117</v>
+      </c>
+      <c r="J26" s="125" t="s">
+        <v>117</v>
+      </c>
+      <c r="K26" s="125" t="s">
+        <v>117</v>
+      </c>
+      <c r="L26" s="125" t="s">
+        <v>117</v>
+      </c>
+      <c r="M26" s="104" t="s">
+        <v>27</v>
+      </c>
+      <c r="N26" s="104" t="s">
+        <v>27</v>
+      </c>
+      <c r="O26" s="125" t="s">
+        <v>117</v>
+      </c>
+      <c r="P26" s="125" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q26" s="85" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A27" s="10" t="s">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A28" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B28" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C28" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E28" s="5">
         <v>766</v>
       </c>
-      <c r="F27" s="17">
+      <c r="F28" s="17">
         <v>1.28252E-2</v>
       </c>
-      <c r="G27" s="17">
+      <c r="G28" s="17">
         <v>2.7534159999999998E-2</v>
       </c>
-      <c r="H27" s="17">
+      <c r="H28" s="17">
         <v>0.46579300000000001</v>
       </c>
-      <c r="I27" s="17">
+      <c r="I28" s="17">
         <v>0.64149999999999996</v>
       </c>
-      <c r="J27" s="17">
+      <c r="J28" s="17">
         <v>-4.1140749999999997E-2</v>
       </c>
-      <c r="K27" s="17">
+      <c r="K28" s="17">
         <v>6.6791181000000005E-2</v>
       </c>
-      <c r="L27" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="M27" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="N27" s="5">
+      <c r="L28" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="M28" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="N28" s="5">
         <v>0.39305909999999999</v>
       </c>
-      <c r="O27" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="P27" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q27" s="5" t="s">
+      <c r="O28" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="P28" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q28" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A28" s="11" t="s">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A29" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B29" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C29" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D29" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E29" s="6">
         <v>127</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F29" s="8">
         <v>0.17732239999999999</v>
       </c>
-      <c r="G28" s="8">
+      <c r="G29" s="8">
         <v>0.14088790000000001</v>
       </c>
-      <c r="H28" s="8">
+      <c r="H29" s="8">
         <v>1.2586059999999999</v>
       </c>
-      <c r="I28" s="8">
+      <c r="I29" s="8">
         <v>0.21049999999999999</v>
       </c>
-      <c r="J28" s="8">
+      <c r="J29" s="8">
         <v>-9.8812860000000002E-2</v>
       </c>
-      <c r="K28" s="8">
+      <c r="K29" s="8">
         <v>0.45345760000000002</v>
       </c>
-      <c r="L28" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="M28" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="N28" s="6">
+      <c r="L29" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="M29" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="N29" s="6">
         <v>0.3511283</v>
       </c>
-      <c r="O28" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="P28" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q28" s="11" t="s">
+      <c r="O29" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="P29" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q29" s="11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="12" t="s">
+    <row r="30" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B30" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C30" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D30" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E30" s="9">
         <v>129</v>
       </c>
-      <c r="F29" s="19">
+      <c r="F30" s="19">
         <v>0.1242379</v>
       </c>
-      <c r="G29" s="19">
+      <c r="G30" s="19">
         <v>6.1530500000000002E-2</v>
       </c>
-      <c r="H29" s="19">
+      <c r="H30" s="19">
         <v>2.0190999999999999</v>
       </c>
-      <c r="I29" s="36">
+      <c r="I30" s="36">
         <v>4.5600000000000002E-2</v>
       </c>
-      <c r="J29" s="19">
+      <c r="J30" s="19">
         <v>3.6402560000000001E-3</v>
       </c>
-      <c r="K29" s="19">
+      <c r="K30" s="19">
         <v>0.24483557</v>
       </c>
-      <c r="L29" s="9" t="s">
+      <c r="L30" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="M29" s="9">
+      <c r="M30" s="9">
         <v>1.7639999999999999E-2</v>
       </c>
-      <c r="N29" s="106" t="s">
-        <v>27</v>
-      </c>
-      <c r="O29" s="106">
+      <c r="N30" s="105" t="s">
+        <v>27</v>
+      </c>
+      <c r="O30" s="105">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="P29" s="106" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q29" s="9" t="s">
+      <c r="P30" s="105" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q30" s="9" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="79" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="78" t="s">
+    <row r="31" spans="1:17" s="79" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="79" t="s">
+      <c r="B31" s="79" t="s">
         <v>112</v>
       </c>
-      <c r="C30" s="79" t="s">
+      <c r="C31" s="79" t="s">
         <v>94</v>
       </c>
-      <c r="D30" s="79" t="s">
+      <c r="D31" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="E30" s="79">
+      <c r="E31" s="79">
         <v>129</v>
       </c>
-      <c r="F30" s="82"/>
-      <c r="G30" s="82"/>
-      <c r="H30" s="82"/>
-      <c r="I30" s="85"/>
-      <c r="J30" s="82"/>
-      <c r="K30" s="82"/>
-      <c r="L30" s="105" t="s">
-        <v>27</v>
-      </c>
-      <c r="M30" s="105" t="s">
-        <v>27</v>
-      </c>
-      <c r="N30" s="105" t="s">
-        <v>27</v>
-      </c>
-      <c r="O30" s="80"/>
-      <c r="P30" s="80"/>
+      <c r="F31" s="82">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="G31" s="82">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="H31" s="82">
+        <v>2.2490000000000001</v>
+      </c>
+      <c r="I31" s="84">
+        <v>2.4500000000000001E-2</v>
+      </c>
+      <c r="J31" s="82">
+        <v>2.0999999999999999E-3</v>
+      </c>
+      <c r="K31" s="82">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="L31" s="104" t="s">
+        <v>27</v>
+      </c>
+      <c r="M31" s="104" t="s">
+        <v>27</v>
+      </c>
+      <c r="N31" s="104" t="s">
+        <v>27</v>
+      </c>
+      <c r="O31" s="82">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="P31" s="82">
+        <v>1.2430000000000001</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4985,9 +5140,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44B5211-D37C-46F5-A2CD-0BEBDDA2FFCE}">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q20" sqref="Q20"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5074,31 +5229,31 @@
       <c r="G2" s="22">
         <v>4.1466999999999997E-3</v>
       </c>
-      <c r="H2" s="121">
+      <c r="H2" s="119">
         <v>0.79335800000000001</v>
       </c>
-      <c r="I2" s="121">
+      <c r="I2" s="119">
         <v>0.42849999999999999</v>
       </c>
       <c r="J2" s="22">
         <v>-4.8375750000000002E-3</v>
       </c>
-      <c r="K2" s="121">
+      <c r="K2" s="119">
         <v>1.141722E-2</v>
       </c>
-      <c r="L2" s="122" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="122" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" s="121">
+      <c r="L2" s="120" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="120" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="119">
         <v>0.79097019999999996</v>
       </c>
-      <c r="O2" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="103" t="s">
+      <c r="O2" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="102" t="s">
         <v>27</v>
       </c>
       <c r="Q2" s="5" t="s">
@@ -5124,34 +5279,34 @@
       <c r="F3" s="23">
         <v>2.9464000000000001E-3</v>
       </c>
-      <c r="G3" s="123">
+      <c r="G3" s="121">
         <v>1.8641999999999999E-2</v>
       </c>
-      <c r="H3" s="123">
+      <c r="H3" s="121">
         <v>0.15804950000000001</v>
       </c>
-      <c r="I3" s="123">
+      <c r="I3" s="121">
         <v>0.87490000000000001</v>
       </c>
-      <c r="J3" s="123">
+      <c r="J3" s="121">
         <v>-3.3591309999999999E-2</v>
       </c>
-      <c r="K3" s="123">
+      <c r="K3" s="121">
         <v>3.9484030000000003E-2</v>
       </c>
-      <c r="L3" s="124" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="124" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3" s="123">
+      <c r="L3" s="122" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="122" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="121">
         <v>0.4</v>
       </c>
-      <c r="O3" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" s="104" t="s">
+      <c r="O3" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" s="103" t="s">
         <v>27</v>
       </c>
       <c r="Q3" s="6" t="s">
@@ -5177,34 +5332,34 @@
       <c r="F4" s="26">
         <v>-8.1607999999999993E-3</v>
       </c>
-      <c r="G4" s="107">
+      <c r="G4" s="106">
         <v>1.2829399999999999E-2</v>
       </c>
-      <c r="H4" s="107">
+      <c r="H4" s="106">
         <v>-0.6361</v>
       </c>
-      <c r="I4" s="107">
+      <c r="I4" s="106">
         <v>0.5272</v>
       </c>
-      <c r="J4" s="107">
+      <c r="J4" s="106">
         <v>-3.3306049999999997E-2</v>
       </c>
-      <c r="K4" s="107">
+      <c r="K4" s="106">
         <v>1.6984369999999999E-2</v>
       </c>
-      <c r="L4" s="107" t="s">
+      <c r="L4" s="106" t="s">
         <v>75</v>
       </c>
-      <c r="M4" s="107">
+      <c r="M4" s="106">
         <v>2.2100000000000002E-2</v>
       </c>
-      <c r="N4" s="125" t="s">
+      <c r="N4" s="123" t="s">
         <v>27</v>
       </c>
       <c r="O4" s="9">
         <v>0.22558120000000001</v>
       </c>
-      <c r="P4" s="117" t="s">
+      <c r="P4" s="116" t="s">
         <v>27</v>
       </c>
       <c r="Q4" s="9" t="s">
@@ -5227,33 +5382,54 @@
       <c r="E5" s="79">
         <v>61</v>
       </c>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
-      <c r="J5" s="99"/>
-      <c r="K5" s="99"/>
-      <c r="L5" s="102" t="s">
-        <v>27</v>
-      </c>
-      <c r="M5" s="102" t="s">
-        <v>27</v>
-      </c>
-      <c r="N5" s="102" t="s">
-        <v>27</v>
+      <c r="F5" s="98">
+        <v>-0.13100000000000001</v>
+      </c>
+      <c r="G5" s="98">
+        <v>0.223</v>
+      </c>
+      <c r="H5" s="98">
+        <v>-0.58799999999999997</v>
+      </c>
+      <c r="I5" s="98">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="J5" s="98">
+        <v>-0.57799999999999996</v>
+      </c>
+      <c r="K5" s="98">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="L5" s="101" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="101" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="101" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5" s="79">
+        <v>4.6600000000000003E-2</v>
+      </c>
+      <c r="P5" s="79">
+        <v>14.879</v>
+      </c>
+      <c r="Q5" s="79" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="13"/>
-      <c r="F6" s="126"/>
-      <c r="G6" s="126"/>
-      <c r="H6" s="126"/>
-      <c r="I6" s="126"/>
-      <c r="J6" s="126"/>
-      <c r="K6" s="126"/>
-      <c r="L6" s="126"/>
-      <c r="M6" s="126"/>
-      <c r="N6" s="126"/>
+      <c r="F6" s="124"/>
+      <c r="G6" s="124"/>
+      <c r="H6" s="124"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="124"/>
+      <c r="M6" s="124"/>
+      <c r="N6" s="124"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
@@ -5274,34 +5450,34 @@
       <c r="F7" s="22">
         <v>-7.9182000000000002E-3</v>
       </c>
-      <c r="G7" s="121">
+      <c r="G7" s="119">
         <v>2.0384699999999999E-2</v>
       </c>
-      <c r="H7" s="121">
+      <c r="H7" s="119">
         <v>-0.38844099999999998</v>
       </c>
-      <c r="I7" s="121">
+      <c r="I7" s="119">
         <v>0.69810000000000005</v>
       </c>
-      <c r="J7" s="121">
+      <c r="J7" s="119">
         <v>-4.7871419999999998E-2</v>
       </c>
-      <c r="K7" s="121">
+      <c r="K7" s="119">
         <v>3.2034960000000001E-2</v>
       </c>
-      <c r="L7" s="122" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" s="122" t="s">
-        <v>27</v>
-      </c>
-      <c r="N7" s="121">
+      <c r="L7" s="120" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="120" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="119">
         <v>0.79504620000000004</v>
       </c>
-      <c r="O7" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="P7" s="103" t="s">
+      <c r="O7" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="P7" s="102" t="s">
         <v>27</v>
       </c>
       <c r="Q7" s="5" t="s">
@@ -5324,37 +5500,37 @@
       <c r="E8" s="6">
         <v>67</v>
       </c>
-      <c r="F8" s="123">
+      <c r="F8" s="121">
         <v>8.4329550000000003E-2</v>
       </c>
-      <c r="G8" s="123">
+      <c r="G8" s="121">
         <v>9.1927599999999998E-2</v>
       </c>
-      <c r="H8" s="123">
+      <c r="H8" s="121">
         <v>0.91734780000000005</v>
       </c>
-      <c r="I8" s="123">
+      <c r="I8" s="121">
         <v>0.3624</v>
       </c>
-      <c r="J8" s="123">
+      <c r="J8" s="121">
         <v>-9.5845169999999993E-2</v>
       </c>
-      <c r="K8" s="123">
+      <c r="K8" s="121">
         <v>0.26450430000000003</v>
       </c>
-      <c r="L8" s="124" t="s">
-        <v>27</v>
-      </c>
-      <c r="M8" s="124" t="s">
-        <v>27</v>
-      </c>
-      <c r="N8" s="123">
+      <c r="L8" s="122" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="122" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8" s="121">
         <v>0.48540030000000001</v>
       </c>
-      <c r="O8" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="P8" s="104" t="s">
+      <c r="O8" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="P8" s="103" t="s">
         <v>27</v>
       </c>
       <c r="Q8" s="6" t="s">
@@ -5377,37 +5553,37 @@
       <c r="E9" s="9">
         <v>61</v>
       </c>
-      <c r="F9" s="107">
+      <c r="F9" s="106">
         <v>4.7405000000000003E-2</v>
       </c>
-      <c r="G9" s="107">
+      <c r="G9" s="106">
         <v>4.3688999999999999E-2</v>
       </c>
-      <c r="H9" s="107">
+      <c r="H9" s="106">
         <v>1.0851</v>
       </c>
-      <c r="I9" s="107">
+      <c r="I9" s="106">
         <v>0.28239999999999998</v>
       </c>
-      <c r="J9" s="107">
+      <c r="J9" s="106">
         <v>-3.8223630000000001E-2</v>
       </c>
-      <c r="K9" s="107">
+      <c r="K9" s="106">
         <v>0.1330327</v>
       </c>
-      <c r="L9" s="107" t="s">
+      <c r="L9" s="106" t="s">
         <v>79</v>
       </c>
-      <c r="M9" s="107">
+      <c r="M9" s="106">
         <v>3.5270000000000003E-2</v>
       </c>
-      <c r="N9" s="125" t="s">
+      <c r="N9" s="123" t="s">
         <v>27</v>
       </c>
       <c r="O9" s="9">
         <v>0.21192050000000001</v>
       </c>
-      <c r="P9" s="117" t="s">
+      <c r="P9" s="116" t="s">
         <v>27</v>
       </c>
       <c r="Q9" s="9" t="s">
@@ -5430,33 +5606,54 @@
       <c r="E10" s="79">
         <v>61</v>
       </c>
-      <c r="F10" s="99"/>
-      <c r="G10" s="99"/>
-      <c r="H10" s="99"/>
-      <c r="I10" s="99"/>
-      <c r="J10" s="99"/>
-      <c r="K10" s="99"/>
-      <c r="L10" s="102" t="s">
-        <v>27</v>
-      </c>
-      <c r="M10" s="102" t="s">
-        <v>27</v>
-      </c>
-      <c r="N10" s="102" t="s">
-        <v>27</v>
+      <c r="F10" s="98">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="G10" s="98">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="H10" s="98">
+        <v>0.871</v>
+      </c>
+      <c r="I10" s="98">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="J10" s="98">
+        <v>-0.307</v>
+      </c>
+      <c r="K10" s="98">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="L10" s="101" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="101" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" s="101" t="s">
+        <v>27</v>
+      </c>
+      <c r="O10" s="79">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="P10" s="79">
+        <v>1.5029999999999999</v>
+      </c>
+      <c r="Q10" s="79" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="13"/>
-      <c r="F11" s="126"/>
-      <c r="G11" s="126"/>
-      <c r="H11" s="126"/>
-      <c r="I11" s="126"/>
-      <c r="J11" s="126"/>
-      <c r="K11" s="126"/>
-      <c r="L11" s="126"/>
-      <c r="M11" s="126"/>
-      <c r="N11" s="126"/>
+      <c r="F11" s="124"/>
+      <c r="G11" s="124"/>
+      <c r="H11" s="124"/>
+      <c r="I11" s="124"/>
+      <c r="J11" s="124"/>
+      <c r="K11" s="124"/>
+      <c r="L11" s="124"/>
+      <c r="M11" s="124"/>
+      <c r="N11" s="124"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
@@ -5477,34 +5674,34 @@
       <c r="F12" s="22">
         <v>3.2689999999999998E-4</v>
       </c>
-      <c r="G12" s="121">
+      <c r="G12" s="119">
         <v>2.5091860000000001E-2</v>
       </c>
-      <c r="H12" s="121">
+      <c r="H12" s="119">
         <v>1.3029000000000001E-2</v>
       </c>
-      <c r="I12" s="121">
+      <c r="I12" s="119">
         <v>0.98960000000000004</v>
       </c>
-      <c r="J12" s="121">
+      <c r="J12" s="119">
         <v>-4.885221E-2</v>
       </c>
-      <c r="K12" s="121">
+      <c r="K12" s="119">
         <v>4.9506070999999999E-2</v>
       </c>
-      <c r="L12" s="122" t="s">
-        <v>27</v>
-      </c>
-      <c r="M12" s="122" t="s">
-        <v>27</v>
-      </c>
-      <c r="N12" s="121">
+      <c r="L12" s="120" t="s">
+        <v>27</v>
+      </c>
+      <c r="M12" s="120" t="s">
+        <v>27</v>
+      </c>
+      <c r="N12" s="119">
         <v>0.38529459999999999</v>
       </c>
-      <c r="O12" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="P12" s="103" t="s">
+      <c r="O12" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="P12" s="102" t="s">
         <v>27</v>
       </c>
       <c r="Q12" s="5" t="s">
@@ -5527,37 +5724,37 @@
       <c r="E13" s="6">
         <v>127</v>
       </c>
-      <c r="F13" s="123">
+      <c r="F13" s="121">
         <v>-8.0268199999999998E-2</v>
       </c>
-      <c r="G13" s="123">
+      <c r="G13" s="121">
         <v>0.14992249999999999</v>
       </c>
-      <c r="H13" s="123">
+      <c r="H13" s="121">
         <v>-0.53539820000000005</v>
       </c>
-      <c r="I13" s="123">
+      <c r="I13" s="121">
         <v>0.59330000000000005</v>
       </c>
-      <c r="J13" s="123">
+      <c r="J13" s="121">
         <v>-0.37411097999999998</v>
       </c>
-      <c r="K13" s="123">
+      <c r="K13" s="121">
         <v>0.2135745</v>
       </c>
-      <c r="L13" s="124" t="s">
-        <v>27</v>
-      </c>
-      <c r="M13" s="124" t="s">
-        <v>27</v>
-      </c>
-      <c r="N13" s="123">
+      <c r="L13" s="122" t="s">
+        <v>27</v>
+      </c>
+      <c r="M13" s="122" t="s">
+        <v>27</v>
+      </c>
+      <c r="N13" s="121">
         <v>0.31911040000000002</v>
       </c>
-      <c r="O13" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="P13" s="104" t="s">
+      <c r="O13" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="P13" s="103" t="s">
         <v>27</v>
       </c>
       <c r="Q13" s="6" t="s">
@@ -5580,37 +5777,37 @@
       <c r="E14" s="9">
         <v>129</v>
       </c>
-      <c r="F14" s="107">
+      <c r="F14" s="106">
         <v>3.1053000000000001E-2</v>
       </c>
-      <c r="G14" s="107">
+      <c r="G14" s="106">
         <v>4.5060999999999997E-2</v>
       </c>
-      <c r="H14" s="107">
+      <c r="H14" s="106">
         <v>0.68910000000000005</v>
       </c>
-      <c r="I14" s="107">
+      <c r="I14" s="106">
         <v>0.49199999999999999</v>
       </c>
-      <c r="J14" s="107">
+      <c r="J14" s="106">
         <v>-5.7265589999999998E-2</v>
       </c>
-      <c r="K14" s="107">
+      <c r="K14" s="106">
         <v>0.11937161</v>
       </c>
-      <c r="L14" s="107" t="s">
+      <c r="L14" s="106" t="s">
         <v>83</v>
       </c>
-      <c r="M14" s="107">
+      <c r="M14" s="106">
         <v>-1.0330000000000001E-2</v>
       </c>
-      <c r="N14" s="125" t="s">
+      <c r="N14" s="123" t="s">
         <v>27</v>
       </c>
       <c r="O14" s="35">
         <v>2.578865E-7</v>
       </c>
-      <c r="P14" s="117" t="s">
+      <c r="P14" s="116" t="s">
         <v>27</v>
       </c>
       <c r="Q14" s="9" t="s">
@@ -5633,34 +5830,53 @@
       <c r="E15" s="79">
         <v>129</v>
       </c>
-      <c r="F15" s="99"/>
-      <c r="G15" s="99"/>
-      <c r="H15" s="99"/>
-      <c r="I15" s="99"/>
-      <c r="J15" s="99"/>
-      <c r="K15" s="99"/>
-      <c r="L15" s="102" t="s">
-        <v>27</v>
-      </c>
-      <c r="M15" s="102" t="s">
-        <v>27</v>
-      </c>
-      <c r="N15" s="102" t="s">
-        <v>27</v>
-      </c>
-      <c r="O15" s="80"/>
-      <c r="P15" s="80"/>
+      <c r="F15" s="98">
+        <v>0.217</v>
+      </c>
+      <c r="G15" s="98">
+        <v>0.188</v>
+      </c>
+      <c r="H15" s="98">
+        <v>1.1539999999999999</v>
+      </c>
+      <c r="I15" s="98">
+        <v>0.248</v>
+      </c>
+      <c r="J15" s="98">
+        <v>-0.14899999999999999</v>
+      </c>
+      <c r="K15" s="98">
+        <v>0.63</v>
+      </c>
+      <c r="L15" s="101" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="101" t="s">
+        <v>27</v>
+      </c>
+      <c r="N15" s="101" t="s">
+        <v>27</v>
+      </c>
+      <c r="O15" s="80">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="P15" s="80">
+        <v>1.2430000000000001</v>
+      </c>
+      <c r="Q15" s="79" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="F16" s="126"/>
-      <c r="G16" s="126"/>
-      <c r="H16" s="126"/>
-      <c r="I16" s="126"/>
-      <c r="J16" s="126"/>
-      <c r="K16" s="126"/>
-      <c r="L16" s="126"/>
-      <c r="M16" s="126"/>
-      <c r="N16" s="126"/>
+      <c r="F16" s="124"/>
+      <c r="G16" s="124"/>
+      <c r="H16" s="124"/>
+      <c r="I16" s="124"/>
+      <c r="J16" s="124"/>
+      <c r="K16" s="124"/>
+      <c r="L16" s="124"/>
+      <c r="M16" s="124"/>
+      <c r="N16" s="124"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
@@ -5678,37 +5894,37 @@
       <c r="E17" s="5">
         <v>766</v>
       </c>
-      <c r="F17" s="121">
+      <c r="F17" s="119">
         <v>2.5092199999999999E-2</v>
       </c>
-      <c r="G17" s="121">
+      <c r="G17" s="119">
         <v>3.9052940000000001E-2</v>
       </c>
-      <c r="H17" s="121">
+      <c r="H17" s="119">
         <v>0.64251800000000003</v>
       </c>
-      <c r="I17" s="121">
+      <c r="I17" s="119">
         <v>0.52070000000000005</v>
       </c>
-      <c r="J17" s="121">
+      <c r="J17" s="119">
         <v>-5.145015E-2</v>
       </c>
-      <c r="K17" s="121">
+      <c r="K17" s="119">
         <v>0.101634554</v>
       </c>
-      <c r="L17" s="122" t="s">
-        <v>27</v>
-      </c>
-      <c r="M17" s="122" t="s">
-        <v>27</v>
-      </c>
-      <c r="N17" s="121">
+      <c r="L17" s="120" t="s">
+        <v>27</v>
+      </c>
+      <c r="M17" s="120" t="s">
+        <v>27</v>
+      </c>
+      <c r="N17" s="119">
         <v>0.38832739999999999</v>
       </c>
-      <c r="O17" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="P17" s="103" t="s">
+      <c r="O17" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="P17" s="102" t="s">
         <v>27</v>
       </c>
       <c r="Q17" s="5" t="s">
@@ -5731,37 +5947,37 @@
       <c r="E18" s="6">
         <v>127</v>
       </c>
-      <c r="F18" s="123">
+      <c r="F18" s="121">
         <v>-1.7120699999999999E-2</v>
       </c>
-      <c r="G18" s="123">
+      <c r="G18" s="121">
         <v>0.17630109999999999</v>
       </c>
-      <c r="H18" s="123">
+      <c r="H18" s="121">
         <v>-9.7110299999999997E-2</v>
       </c>
-      <c r="I18" s="123">
+      <c r="I18" s="121">
         <v>0.92279999999999995</v>
       </c>
-      <c r="J18" s="123">
+      <c r="J18" s="121">
         <v>-0.36266453999999998</v>
       </c>
-      <c r="K18" s="123">
+      <c r="K18" s="121">
         <v>0.32842320000000003</v>
       </c>
-      <c r="L18" s="124" t="s">
-        <v>27</v>
-      </c>
-      <c r="M18" s="124" t="s">
-        <v>27</v>
-      </c>
-      <c r="N18" s="123">
+      <c r="L18" s="122" t="s">
+        <v>27</v>
+      </c>
+      <c r="M18" s="122" t="s">
+        <v>27</v>
+      </c>
+      <c r="N18" s="121">
         <v>0.34039550000000002</v>
       </c>
-      <c r="O18" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="P18" s="104" t="s">
+      <c r="O18" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="P18" s="103" t="s">
         <v>27</v>
       </c>
       <c r="Q18" s="6" t="s">
@@ -5784,37 +6000,37 @@
       <c r="E19" s="9">
         <v>129</v>
       </c>
-      <c r="F19" s="107">
+      <c r="F19" s="106">
         <v>7.3262999999999995E-2</v>
       </c>
-      <c r="G19" s="107">
+      <c r="G19" s="106">
         <v>8.2063999999999998E-2</v>
       </c>
-      <c r="H19" s="107">
+      <c r="H19" s="106">
         <v>0.89280000000000004</v>
       </c>
-      <c r="I19" s="107">
+      <c r="I19" s="106">
         <v>0.37369000000000002</v>
       </c>
-      <c r="J19" s="107">
+      <c r="J19" s="106">
         <v>-8.757935E-2</v>
       </c>
-      <c r="K19" s="107">
+      <c r="K19" s="106">
         <v>0.23410527</v>
       </c>
-      <c r="L19" s="107" t="s">
+      <c r="L19" s="106" t="s">
         <v>85</v>
       </c>
-      <c r="M19" s="107">
+      <c r="M19" s="106">
         <v>-7.7679999999999997E-3</v>
       </c>
-      <c r="N19" s="125" t="s">
+      <c r="N19" s="123" t="s">
         <v>27</v>
       </c>
       <c r="O19" s="35">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="P19" s="117" t="s">
+      <c r="P19" s="116" t="s">
         <v>27</v>
       </c>
       <c r="Q19" s="9" t="s">
@@ -5837,20 +6053,41 @@
       <c r="E20" s="79">
         <v>129</v>
       </c>
-      <c r="F20" s="99"/>
-      <c r="G20" s="99"/>
-      <c r="H20" s="99"/>
-      <c r="I20" s="99"/>
-      <c r="J20" s="99"/>
-      <c r="K20" s="99"/>
-      <c r="L20" s="102" t="s">
-        <v>27</v>
-      </c>
-      <c r="M20" s="102" t="s">
-        <v>27</v>
-      </c>
-      <c r="N20" s="102" t="s">
-        <v>27</v>
+      <c r="F20" s="98">
+        <v>0.156</v>
+      </c>
+      <c r="G20" s="98">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="H20" s="98">
+        <v>0.86</v>
+      </c>
+      <c r="I20" s="82">
+        <v>0.38979999999999998</v>
+      </c>
+      <c r="J20" s="98">
+        <v>-0.20100000000000001</v>
+      </c>
+      <c r="K20" s="98">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="L20" s="101" t="s">
+        <v>27</v>
+      </c>
+      <c r="M20" s="101" t="s">
+        <v>27</v>
+      </c>
+      <c r="N20" s="101" t="s">
+        <v>27</v>
+      </c>
+      <c r="O20" s="79">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="P20" s="79">
+        <v>1.2010000000000001</v>
+      </c>
+      <c r="Q20" s="79" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -5864,7 +6101,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R5" sqref="R5"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5960,19 +6197,19 @@
       <c r="K2" s="22">
         <v>9.1120610000000005E-4</v>
       </c>
-      <c r="L2" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="103" t="s">
+      <c r="L2" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="102" t="s">
         <v>27</v>
       </c>
       <c r="N2" s="5">
         <v>0.37407960000000001</v>
       </c>
-      <c r="O2" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="103" t="s">
+      <c r="O2" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="102" t="s">
         <v>27</v>
       </c>
       <c r="Q2" s="5" t="s">
@@ -6013,19 +6250,19 @@
       <c r="K3" s="6">
         <v>0.19874919999999999</v>
       </c>
-      <c r="L3" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="104" t="s">
+      <c r="L3" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="103" t="s">
         <v>27</v>
       </c>
       <c r="N3" s="6">
         <v>0.2487848</v>
       </c>
-      <c r="O3" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" s="104" t="s">
+      <c r="O3" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" s="103" t="s">
         <v>27</v>
       </c>
       <c r="Q3" s="6" t="s">
@@ -6072,13 +6309,13 @@
       <c r="M4" s="9">
         <v>-9.7959999999999992E-3</v>
       </c>
-      <c r="N4" s="106" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" s="106">
+      <c r="N4" s="105" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" s="105">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="P4" s="106" t="s">
+      <c r="P4" s="105" t="s">
         <v>27</v>
       </c>
       <c r="Q4" s="9" t="s">
@@ -6101,23 +6338,42 @@
       <c r="E5" s="79">
         <v>122</v>
       </c>
-      <c r="F5" s="82"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="82"/>
-      <c r="I5" s="82"/>
-      <c r="J5" s="82"/>
-      <c r="K5" s="82"/>
-      <c r="L5" s="105" t="s">
-        <v>27</v>
-      </c>
-      <c r="M5" s="105" t="s">
-        <v>27</v>
-      </c>
-      <c r="N5" s="105" t="s">
-        <v>27</v>
-      </c>
-      <c r="O5" s="99"/>
-      <c r="P5" s="82"/>
+      <c r="F5" s="82">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="G5" s="82">
+        <v>0.224</v>
+      </c>
+      <c r="H5" s="82">
+        <v>1.4650000000000001</v>
+      </c>
+      <c r="I5" s="82">
+        <v>0.1429</v>
+      </c>
+      <c r="J5" s="82">
+        <v>-0.109</v>
+      </c>
+      <c r="K5" s="82">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="L5" s="104" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="104" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="104" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5" s="98">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="P5" s="82">
+        <v>1.363</v>
+      </c>
+      <c r="Q5" s="79" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="13"/>
@@ -6156,19 +6412,19 @@
       <c r="K7" s="5">
         <v>0.32617759950000003</v>
       </c>
-      <c r="L7" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" s="103" t="s">
+      <c r="L7" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="102" t="s">
         <v>27</v>
       </c>
       <c r="N7" s="5">
         <v>0.38720739999999998</v>
       </c>
-      <c r="O7" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="P7" s="103" t="s">
+      <c r="O7" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="P7" s="102" t="s">
         <v>27</v>
       </c>
       <c r="Q7" s="5" t="s">
@@ -6209,19 +6465,19 @@
       <c r="K8" s="37">
         <v>2.7966720999999999</v>
       </c>
-      <c r="L8" s="116" t="s">
-        <v>27</v>
-      </c>
-      <c r="M8" s="116" t="s">
+      <c r="L8" s="115" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="115" t="s">
         <v>27</v>
       </c>
       <c r="N8" s="37">
         <v>0.2152647</v>
       </c>
-      <c r="O8" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="P8" s="104" t="s">
+      <c r="O8" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="P8" s="103" t="s">
         <v>27</v>
       </c>
       <c r="Q8" s="37" t="s">
@@ -6268,13 +6524,13 @@
       <c r="M9" s="39">
         <v>4.2430000000000002E-2</v>
       </c>
-      <c r="N9" s="115" t="s">
-        <v>27</v>
-      </c>
-      <c r="O9" s="115">
+      <c r="N9" s="114" t="s">
+        <v>27</v>
+      </c>
+      <c r="O9" s="114">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="P9" s="115" t="s">
+      <c r="P9" s="114" t="s">
         <v>27</v>
       </c>
       <c r="Q9" s="39" t="s">
@@ -6285,54 +6541,52 @@
       <c r="A10" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="86" t="s">
+      <c r="B10" s="85" t="s">
         <v>112</v>
       </c>
-      <c r="C10" s="86" t="s">
+      <c r="C10" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="86" t="s">
+      <c r="D10" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="86">
+      <c r="E10" s="85">
         <v>129</v>
       </c>
-      <c r="F10" s="127" t="s">
-        <v>118</v>
-      </c>
-      <c r="G10" s="127" t="s">
-        <v>118</v>
-      </c>
-      <c r="H10" s="127" t="s">
-        <v>118</v>
-      </c>
-      <c r="I10" s="127" t="s">
-        <v>118</v>
-      </c>
-      <c r="J10" s="127" t="s">
-        <v>118</v>
-      </c>
-      <c r="K10" s="127" t="s">
-        <v>118</v>
-      </c>
-      <c r="L10" s="127" t="s">
-        <v>118</v>
-      </c>
-      <c r="M10" s="105" t="s">
-        <v>27</v>
-      </c>
-      <c r="N10" s="105" t="s">
-        <v>27</v>
-      </c>
-      <c r="O10" s="127" t="s">
-        <v>118</v>
-      </c>
-      <c r="P10" s="127" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q10" s="86" t="s">
+      <c r="F10" s="125" t="s">
         <v>117</v>
       </c>
+      <c r="G10" s="125" t="s">
+        <v>117</v>
+      </c>
+      <c r="H10" s="125" t="s">
+        <v>117</v>
+      </c>
+      <c r="I10" s="125" t="s">
+        <v>117</v>
+      </c>
+      <c r="J10" s="125" t="s">
+        <v>117</v>
+      </c>
+      <c r="K10" s="125" t="s">
+        <v>117</v>
+      </c>
+      <c r="L10" s="125" t="s">
+        <v>117</v>
+      </c>
+      <c r="M10" s="104" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" s="104" t="s">
+        <v>27</v>
+      </c>
+      <c r="O10" s="125" t="s">
+        <v>117</v>
+      </c>
+      <c r="P10" s="125" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q10" s="85"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="13"/>
@@ -6443,19 +6697,19 @@
       <c r="K2" s="17">
         <v>8.6904349999999998E-3</v>
       </c>
-      <c r="L2" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="103" t="s">
+      <c r="L2" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="102" t="s">
         <v>27</v>
       </c>
       <c r="N2" s="5">
         <v>0.35023149999999997</v>
       </c>
-      <c r="O2" s="103" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="103" t="s">
+      <c r="O2" s="102" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="102" t="s">
         <v>27</v>
       </c>
       <c r="Q2" s="5" t="s">
@@ -6496,19 +6750,19 @@
       <c r="K3" s="8">
         <v>0.32626369999999999</v>
       </c>
-      <c r="L3" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="104" t="s">
+      <c r="L3" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="103" t="s">
         <v>27</v>
       </c>
       <c r="N3" s="6">
         <v>0.29118569999999999</v>
       </c>
-      <c r="O3" s="104" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" s="104" t="s">
+      <c r="O3" s="103" t="s">
+        <v>27</v>
+      </c>
+      <c r="P3" s="103" t="s">
         <v>27</v>
       </c>
       <c r="Q3" s="6" t="s">
@@ -6555,13 +6809,13 @@
       <c r="M4" s="19">
         <v>-6.1570000000000001E-3</v>
       </c>
-      <c r="N4" s="106" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" s="106">
+      <c r="N4" s="105" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" s="105">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="P4" s="106" t="s">
+      <c r="P4" s="105" t="s">
         <v>27</v>
       </c>
       <c r="Q4" s="9" t="s">
@@ -6602,13 +6856,13 @@
       <c r="K5" s="82">
         <v>0.40899999999999997</v>
       </c>
-      <c r="L5" s="105" t="s">
-        <v>27</v>
-      </c>
-      <c r="M5" s="105" t="s">
-        <v>27</v>
-      </c>
-      <c r="N5" s="105" t="s">
+      <c r="L5" s="104" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="104" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="104" t="s">
         <v>27</v>
       </c>
       <c r="O5" s="82">
@@ -6617,8 +6871,8 @@
       <c r="P5" s="80">
         <v>1.244</v>
       </c>
-      <c r="Q5" s="128" t="s">
-        <v>119</v>
+      <c r="Q5" s="126" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">

</xml_diff>